<commit_message>
menus, popups, image manager
</commit_message>
<xml_diff>
--- a/application/import_data/menus.xlsx
+++ b/application/import_data/menus.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221" codeName="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26408" codeName="{00000000-0000-0000-0000-000000000000}"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mneucollins/Sites/PWM/resources/csv/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="7460" yWindow="1100" windowWidth="25600" windowHeight="14560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="menus" sheetId="2" r:id="rId1"/>
@@ -1325,6 +1330,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1653,11 +1663,11 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="1"/>
     <col min="2" max="2" width="16" style="1" customWidth="1"/>
@@ -1667,7 +1677,7 @@
     <col min="6" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
@@ -1684,7 +1694,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>100</v>
       </c>
@@ -1701,7 +1711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>200</v>
       </c>
@@ -1718,7 +1728,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>6065</v>
       </c>
@@ -1735,7 +1745,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>6043</v>
       </c>
@@ -1752,7 +1762,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="7">
         <v>6071</v>
       </c>
@@ -1769,7 +1779,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>6036</v>
       </c>
@@ -1786,7 +1796,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="7">
         <v>6002</v>
       </c>
@@ -1803,7 +1813,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="7">
         <v>6056</v>
       </c>
@@ -1820,7 +1830,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
         <v>6108</v>
       </c>
@@ -1837,7 +1847,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
         <v>6053</v>
       </c>
@@ -1851,7 +1861,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="1">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1861,11 +1871,6 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1879,7 +1884,7 @@
       <selection pane="bottomLeft" activeCell="G201" sqref="G201"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.6640625" style="4" bestFit="1" customWidth="1"/>
@@ -1893,7 +1898,7 @@
     <col min="10" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -1922,7 +1927,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>1000</v>
       </c>
@@ -1947,7 +1952,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>2000</v>
       </c>
@@ -1970,7 +1975,7 @@
       </c>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>3000</v>
       </c>
@@ -1993,7 +1998,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>3400</v>
       </c>
@@ -2020,7 +2025,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>3004</v>
       </c>
@@ -2047,7 +2052,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>3006</v>
       </c>
@@ -2074,7 +2079,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>3415</v>
       </c>
@@ -2101,7 +2106,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>3420</v>
       </c>
@@ -2128,7 +2133,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>3425</v>
       </c>
@@ -2155,7 +2160,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>3430</v>
       </c>
@@ -2182,7 +2187,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>3435</v>
       </c>
@@ -2209,7 +2214,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>3440</v>
       </c>
@@ -2234,7 +2239,7 @@
       </c>
       <c r="I13" s="5"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>3445</v>
       </c>
@@ -2259,7 +2264,7 @@
       </c>
       <c r="I14" s="5"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>3450</v>
       </c>
@@ -2284,7 +2289,7 @@
       </c>
       <c r="I15" s="5"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <v>3455</v>
       </c>
@@ -2311,7 +2316,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <v>3010</v>
       </c>
@@ -2338,7 +2343,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <v>3100</v>
       </c>
@@ -2363,7 +2368,7 @@
       </c>
       <c r="I18" s="5"/>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <v>3110</v>
       </c>
@@ -2388,7 +2393,7 @@
       </c>
       <c r="I19" s="5"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="5">
         <v>3120</v>
       </c>
@@ -2413,7 +2418,7 @@
       </c>
       <c r="I20" s="5"/>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
         <v>3130</v>
       </c>
@@ -2438,7 +2443,7 @@
       </c>
       <c r="I21" s="5"/>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="5">
         <v>3140</v>
       </c>
@@ -2463,7 +2468,7 @@
       </c>
       <c r="I22" s="5"/>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="5">
         <v>3150</v>
       </c>
@@ -2488,7 +2493,7 @@
       </c>
       <c r="I23" s="5"/>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="5">
         <v>3200</v>
       </c>
@@ -2513,7 +2518,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="5">
         <v>3210</v>
       </c>
@@ -2538,7 +2543,7 @@
       </c>
       <c r="I25" s="5"/>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
         <v>3220</v>
       </c>
@@ -2563,7 +2568,7 @@
       </c>
       <c r="I26" s="5"/>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
         <v>3230</v>
       </c>
@@ -2588,7 +2593,7 @@
       </c>
       <c r="I27" s="5"/>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="5">
         <v>3240</v>
       </c>
@@ -2613,7 +2618,7 @@
       </c>
       <c r="I28" s="5"/>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="5">
         <v>3300</v>
       </c>
@@ -2638,7 +2643,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="5">
         <v>3310</v>
       </c>
@@ -2663,7 +2668,7 @@
       </c>
       <c r="I30" s="5"/>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="5">
         <v>3320</v>
       </c>
@@ -2688,7 +2693,7 @@
       </c>
       <c r="I31" s="5"/>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="5">
         <v>3330</v>
       </c>
@@ -2713,7 +2718,7 @@
       </c>
       <c r="I32" s="5"/>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="5">
         <v>3340</v>
       </c>
@@ -2738,7 +2743,7 @@
       </c>
       <c r="I33" s="5"/>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="5">
         <v>3350</v>
       </c>
@@ -2763,7 +2768,7 @@
       </c>
       <c r="I34" s="5"/>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
         <v>4000</v>
       </c>
@@ -2786,7 +2791,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="5">
         <v>4100</v>
       </c>
@@ -2811,7 +2816,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="5">
         <v>4120</v>
       </c>
@@ -2838,7 +2843,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="5">
         <v>4130</v>
       </c>
@@ -2865,7 +2870,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="5">
         <v>4140</v>
       </c>
@@ -2890,7 +2895,7 @@
       </c>
       <c r="I39" s="5"/>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="5">
         <v>4150</v>
       </c>
@@ -2917,7 +2922,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="5">
         <v>4160</v>
       </c>
@@ -2942,7 +2947,7 @@
       </c>
       <c r="I41" s="5"/>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="5">
         <v>4170</v>
       </c>
@@ -2969,7 +2974,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="5">
         <v>4200</v>
       </c>
@@ -2994,7 +2999,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="5">
         <v>4210</v>
       </c>
@@ -3019,7 +3024,7 @@
       </c>
       <c r="I44" s="5"/>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="5">
         <v>4220</v>
       </c>
@@ -3044,7 +3049,7 @@
       </c>
       <c r="I45" s="5"/>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="5">
         <v>4300</v>
       </c>
@@ -3069,7 +3074,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="5">
         <v>4310</v>
       </c>
@@ -3094,7 +3099,7 @@
       </c>
       <c r="I47" s="5"/>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="5">
         <v>4320</v>
       </c>
@@ -3119,7 +3124,7 @@
       </c>
       <c r="I48" s="5"/>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="5">
         <v>5000</v>
       </c>
@@ -3144,7 +3149,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="6">
         <v>6000</v>
       </c>
@@ -3165,7 +3170,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="6">
         <v>6001</v>
       </c>
@@ -3186,7 +3191,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="7">
         <v>6002</v>
       </c>
@@ -3211,7 +3216,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="7">
         <v>6003</v>
       </c>
@@ -3234,7 +3239,7 @@
       <c r="H53" s="7"/>
       <c r="I53" s="7"/>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="7">
         <v>6004</v>
       </c>
@@ -3257,7 +3262,7 @@
       <c r="H54" s="7"/>
       <c r="I54" s="7"/>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="7">
         <v>6005</v>
       </c>
@@ -3280,7 +3285,7 @@
       <c r="H55" s="7"/>
       <c r="I55" s="7"/>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="7">
         <v>6006</v>
       </c>
@@ -3303,7 +3308,7 @@
       <c r="H56" s="7"/>
       <c r="I56" s="7"/>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="7">
         <v>6007</v>
       </c>
@@ -3326,7 +3331,7 @@
       <c r="H57" s="7"/>
       <c r="I57" s="7"/>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="7">
         <v>6008</v>
       </c>
@@ -3349,7 +3354,7 @@
       <c r="H58" s="7"/>
       <c r="I58" s="7"/>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="7">
         <v>6009</v>
       </c>
@@ -3372,7 +3377,7 @@
       <c r="H59" s="7"/>
       <c r="I59" s="7"/>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="7">
         <v>6010</v>
       </c>
@@ -3395,7 +3400,7 @@
       <c r="H60" s="7"/>
       <c r="I60" s="7"/>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="7">
         <v>6011</v>
       </c>
@@ -3418,7 +3423,7 @@
       <c r="H61" s="7"/>
       <c r="I61" s="7"/>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="7">
         <v>6012</v>
       </c>
@@ -3441,7 +3446,7 @@
       <c r="H62" s="7"/>
       <c r="I62" s="7"/>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="7">
         <v>6013</v>
       </c>
@@ -3464,7 +3469,7 @@
       <c r="H63" s="7"/>
       <c r="I63" s="7"/>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="6">
         <v>6014</v>
       </c>
@@ -3483,7 +3488,7 @@
       <c r="H64" s="6"/>
       <c r="I64" s="6"/>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="7">
         <v>6015</v>
       </c>
@@ -3506,7 +3511,7 @@
       <c r="H65" s="7"/>
       <c r="I65" s="7"/>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="7">
         <v>6016</v>
       </c>
@@ -3529,7 +3534,7 @@
       <c r="H66" s="7"/>
       <c r="I66" s="7"/>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="7">
         <v>6017</v>
       </c>
@@ -3552,7 +3557,7 @@
       <c r="H67" s="7"/>
       <c r="I67" s="7"/>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="7">
         <v>6018</v>
       </c>
@@ -3575,7 +3580,7 @@
       <c r="H68" s="7"/>
       <c r="I68" s="7"/>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="7">
         <v>6019</v>
       </c>
@@ -3598,7 +3603,7 @@
       <c r="H69" s="7"/>
       <c r="I69" s="7"/>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="7">
         <v>6020</v>
       </c>
@@ -3621,7 +3626,7 @@
       <c r="H70" s="7"/>
       <c r="I70" s="7"/>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="7">
         <v>6021</v>
       </c>
@@ -3644,7 +3649,7 @@
       <c r="H71" s="7"/>
       <c r="I71" s="7"/>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="7">
         <v>6022</v>
       </c>
@@ -3667,7 +3672,7 @@
       <c r="H72" s="7"/>
       <c r="I72" s="7"/>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="7">
         <v>6023</v>
       </c>
@@ -3690,7 +3695,7 @@
       <c r="H73" s="7"/>
       <c r="I73" s="7"/>
     </row>
-    <row r="74" spans="1:9">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="7">
         <v>6024</v>
       </c>
@@ -3713,7 +3718,7 @@
       <c r="H74" s="7"/>
       <c r="I74" s="7"/>
     </row>
-    <row r="75" spans="1:9">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="7">
         <v>6025</v>
       </c>
@@ -3736,7 +3741,7 @@
       <c r="H75" s="7"/>
       <c r="I75" s="7"/>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="6">
         <v>6026</v>
       </c>
@@ -3755,7 +3760,7 @@
       <c r="H76" s="6"/>
       <c r="I76" s="6"/>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="7">
         <v>6027</v>
       </c>
@@ -3778,7 +3783,7 @@
       <c r="H77" s="7"/>
       <c r="I77" s="7"/>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="7">
         <v>6028</v>
       </c>
@@ -3801,7 +3806,7 @@
       <c r="H78" s="7"/>
       <c r="I78" s="7"/>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="7">
         <v>6029</v>
       </c>
@@ -3824,7 +3829,7 @@
       <c r="H79" s="7"/>
       <c r="I79" s="7"/>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" s="7">
         <v>6030</v>
       </c>
@@ -3847,7 +3852,7 @@
       <c r="H80" s="7"/>
       <c r="I80" s="7"/>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" s="7">
         <v>6031</v>
       </c>
@@ -3870,7 +3875,7 @@
       <c r="H81" s="7"/>
       <c r="I81" s="7"/>
     </row>
-    <row r="82" spans="1:9">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" s="7">
         <v>6032</v>
       </c>
@@ -3893,7 +3898,7 @@
       <c r="H82" s="7"/>
       <c r="I82" s="7"/>
     </row>
-    <row r="83" spans="1:9">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="7">
         <v>6033</v>
       </c>
@@ -3916,7 +3921,7 @@
       <c r="H83" s="7"/>
       <c r="I83" s="7"/>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="6">
         <v>6034</v>
       </c>
@@ -3937,7 +3942,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="7">
         <v>6035</v>
       </c>
@@ -3960,7 +3965,7 @@
       <c r="H85" s="7"/>
       <c r="I85" s="7"/>
     </row>
-    <row r="86" spans="1:9">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" s="7">
         <v>6036</v>
       </c>
@@ -3985,7 +3990,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="87" spans="1:9">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" s="7">
         <v>6037</v>
       </c>
@@ -4008,7 +4013,7 @@
       <c r="H87" s="7"/>
       <c r="I87" s="7"/>
     </row>
-    <row r="88" spans="1:9">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" s="7">
         <v>6038</v>
       </c>
@@ -4031,7 +4036,7 @@
       <c r="H88" s="7"/>
       <c r="I88" s="7"/>
     </row>
-    <row r="89" spans="1:9">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" s="7">
         <v>6039</v>
       </c>
@@ -4054,7 +4059,7 @@
       <c r="H89" s="7"/>
       <c r="I89" s="7"/>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" s="7">
         <v>6040</v>
       </c>
@@ -4077,7 +4082,7 @@
       <c r="H90" s="7"/>
       <c r="I90" s="7"/>
     </row>
-    <row r="91" spans="1:9">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" s="7">
         <v>6041</v>
       </c>
@@ -4100,7 +4105,7 @@
       <c r="H91" s="7"/>
       <c r="I91" s="7"/>
     </row>
-    <row r="92" spans="1:9">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" s="7">
         <v>6042</v>
       </c>
@@ -4123,7 +4128,7 @@
       <c r="H92" s="7"/>
       <c r="I92" s="7"/>
     </row>
-    <row r="93" spans="1:9">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" s="7">
         <v>6043</v>
       </c>
@@ -4148,7 +4153,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="94" spans="1:9">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" s="7">
         <v>6044</v>
       </c>
@@ -4171,7 +4176,7 @@
       <c r="H94" s="7"/>
       <c r="I94" s="7"/>
     </row>
-    <row r="95" spans="1:9">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" s="7">
         <v>6045</v>
       </c>
@@ -4194,7 +4199,7 @@
       <c r="H95" s="7"/>
       <c r="I95" s="7"/>
     </row>
-    <row r="96" spans="1:9">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" s="7">
         <v>6046</v>
       </c>
@@ -4217,7 +4222,7 @@
       <c r="H96" s="7"/>
       <c r="I96" s="7"/>
     </row>
-    <row r="97" spans="1:9">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" s="6">
         <v>6047</v>
       </c>
@@ -4238,7 +4243,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="98" spans="1:9">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" s="7">
         <v>6048</v>
       </c>
@@ -4261,7 +4266,7 @@
       <c r="H98" s="7"/>
       <c r="I98" s="7"/>
     </row>
-    <row r="99" spans="1:9">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" s="7">
         <v>6049</v>
       </c>
@@ -4284,7 +4289,7 @@
       <c r="H99" s="7"/>
       <c r="I99" s="7"/>
     </row>
-    <row r="100" spans="1:9">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" s="7">
         <v>6050</v>
       </c>
@@ -4307,7 +4312,7 @@
       <c r="H100" s="7"/>
       <c r="I100" s="7"/>
     </row>
-    <row r="101" spans="1:9">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" s="7">
         <v>6051</v>
       </c>
@@ -4330,7 +4335,7 @@
       <c r="H101" s="7"/>
       <c r="I101" s="7"/>
     </row>
-    <row r="102" spans="1:9">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" s="7">
         <v>6052</v>
       </c>
@@ -4353,7 +4358,7 @@
       <c r="H102" s="7"/>
       <c r="I102" s="7"/>
     </row>
-    <row r="103" spans="1:9">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" s="7">
         <v>6053</v>
       </c>
@@ -4378,7 +4383,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="104" spans="1:9">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" s="7">
         <v>6054</v>
       </c>
@@ -4401,7 +4406,7 @@
       <c r="H104" s="7"/>
       <c r="I104" s="7"/>
     </row>
-    <row r="105" spans="1:9">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" s="7">
         <v>6055</v>
       </c>
@@ -4424,7 +4429,7 @@
       <c r="H105" s="7"/>
       <c r="I105" s="7"/>
     </row>
-    <row r="106" spans="1:9">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" s="7">
         <v>6056</v>
       </c>
@@ -4449,7 +4454,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="107" spans="1:9">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" s="7">
         <v>6057</v>
       </c>
@@ -4472,7 +4477,7 @@
       <c r="H107" s="7"/>
       <c r="I107" s="7"/>
     </row>
-    <row r="108" spans="1:9">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" s="6">
         <v>6058</v>
       </c>
@@ -4493,7 +4498,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="109" spans="1:9">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" s="7">
         <v>6059</v>
       </c>
@@ -4516,7 +4521,7 @@
       <c r="H109" s="7"/>
       <c r="I109" s="7"/>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" s="7">
         <v>6060</v>
       </c>
@@ -4539,7 +4544,7 @@
       <c r="H110" s="7"/>
       <c r="I110" s="7"/>
     </row>
-    <row r="111" spans="1:9">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" s="7">
         <v>6061</v>
       </c>
@@ -4562,7 +4567,7 @@
       <c r="H111" s="7"/>
       <c r="I111" s="7"/>
     </row>
-    <row r="112" spans="1:9">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" s="7">
         <v>6062</v>
       </c>
@@ -4585,7 +4590,7 @@
       <c r="H112" s="7"/>
       <c r="I112" s="7"/>
     </row>
-    <row r="113" spans="1:9">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" s="7">
         <v>6063</v>
       </c>
@@ -4608,7 +4613,7 @@
       <c r="H113" s="7"/>
       <c r="I113" s="7"/>
     </row>
-    <row r="114" spans="1:9">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A114" s="7">
         <v>6064</v>
       </c>
@@ -4631,7 +4636,7 @@
       <c r="H114" s="7"/>
       <c r="I114" s="7"/>
     </row>
-    <row r="115" spans="1:9">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115" s="7">
         <v>6065</v>
       </c>
@@ -4656,7 +4661,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="116" spans="1:9">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A116" s="7">
         <v>6066</v>
       </c>
@@ -4679,7 +4684,7 @@
       <c r="H116" s="7"/>
       <c r="I116" s="7"/>
     </row>
-    <row r="117" spans="1:9">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A117" s="7">
         <v>6067</v>
       </c>
@@ -4702,7 +4707,7 @@
       <c r="H117" s="7"/>
       <c r="I117" s="7"/>
     </row>
-    <row r="118" spans="1:9">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A118" s="7">
         <v>6068</v>
       </c>
@@ -4725,7 +4730,7 @@
       <c r="H118" s="7"/>
       <c r="I118" s="7"/>
     </row>
-    <row r="119" spans="1:9">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A119" s="7">
         <v>6069</v>
       </c>
@@ -4748,7 +4753,7 @@
       <c r="H119" s="7"/>
       <c r="I119" s="7"/>
     </row>
-    <row r="120" spans="1:9">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A120" s="7">
         <v>6070</v>
       </c>
@@ -4771,7 +4776,7 @@
       <c r="H120" s="7"/>
       <c r="I120" s="7"/>
     </row>
-    <row r="121" spans="1:9">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A121" s="7">
         <v>6071</v>
       </c>
@@ -4796,7 +4801,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="122" spans="1:9">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A122" s="7">
         <v>6072</v>
       </c>
@@ -4819,7 +4824,7 @@
       <c r="H122" s="7"/>
       <c r="I122" s="7"/>
     </row>
-    <row r="123" spans="1:9">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A123" s="7">
         <v>6073</v>
       </c>
@@ -4842,7 +4847,7 @@
       <c r="H123" s="7"/>
       <c r="I123" s="7"/>
     </row>
-    <row r="124" spans="1:9">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A124" s="7">
         <v>6074</v>
       </c>
@@ -4865,7 +4870,7 @@
       <c r="H124" s="7"/>
       <c r="I124" s="7"/>
     </row>
-    <row r="125" spans="1:9">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A125" s="6">
         <v>6075</v>
       </c>
@@ -4884,7 +4889,7 @@
       <c r="H125" s="6"/>
       <c r="I125" s="6"/>
     </row>
-    <row r="126" spans="1:9">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A126" s="7">
         <v>6076</v>
       </c>
@@ -4907,7 +4912,7 @@
       <c r="H126" s="7"/>
       <c r="I126" s="7"/>
     </row>
-    <row r="127" spans="1:9">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A127" s="7">
         <v>6077</v>
       </c>
@@ -4930,7 +4935,7 @@
       <c r="H127" s="7"/>
       <c r="I127" s="7"/>
     </row>
-    <row r="128" spans="1:9">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A128" s="7">
         <v>6078</v>
       </c>
@@ -4953,7 +4958,7 @@
       <c r="H128" s="7"/>
       <c r="I128" s="7"/>
     </row>
-    <row r="129" spans="1:9">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A129" s="7">
         <v>6079</v>
       </c>
@@ -4976,7 +4981,7 @@
       <c r="H129" s="7"/>
       <c r="I129" s="7"/>
     </row>
-    <row r="130" spans="1:9">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A130" s="7">
         <v>6080</v>
       </c>
@@ -4999,7 +5004,7 @@
       <c r="H130" s="7"/>
       <c r="I130" s="7"/>
     </row>
-    <row r="131" spans="1:9">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A131" s="7">
         <v>6081</v>
       </c>
@@ -5022,7 +5027,7 @@
       <c r="H131" s="7"/>
       <c r="I131" s="7"/>
     </row>
-    <row r="132" spans="1:9">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A132" s="7">
         <v>6082</v>
       </c>
@@ -5045,7 +5050,7 @@
       <c r="H132" s="7"/>
       <c r="I132" s="7"/>
     </row>
-    <row r="133" spans="1:9">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A133" s="7">
         <v>6083</v>
       </c>
@@ -5068,7 +5073,7 @@
       <c r="H133" s="7"/>
       <c r="I133" s="7"/>
     </row>
-    <row r="134" spans="1:9">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A134" s="7">
         <v>6084</v>
       </c>
@@ -5091,7 +5096,7 @@
       <c r="H134" s="7"/>
       <c r="I134" s="7"/>
     </row>
-    <row r="135" spans="1:9">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A135" s="6">
         <v>6085</v>
       </c>
@@ -5110,7 +5115,7 @@
       <c r="H135" s="6"/>
       <c r="I135" s="6"/>
     </row>
-    <row r="136" spans="1:9">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A136" s="7">
         <v>6086</v>
       </c>
@@ -5133,7 +5138,7 @@
       <c r="H136" s="7"/>
       <c r="I136" s="7"/>
     </row>
-    <row r="137" spans="1:9">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A137" s="7">
         <v>6087</v>
       </c>
@@ -5156,7 +5161,7 @@
       <c r="H137" s="7"/>
       <c r="I137" s="7"/>
     </row>
-    <row r="138" spans="1:9">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A138" s="7">
         <v>6088</v>
       </c>
@@ -5179,7 +5184,7 @@
       <c r="H138" s="7"/>
       <c r="I138" s="7"/>
     </row>
-    <row r="139" spans="1:9">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A139" s="7">
         <v>6089</v>
       </c>
@@ -5202,7 +5207,7 @@
       <c r="H139" s="7"/>
       <c r="I139" s="7"/>
     </row>
-    <row r="140" spans="1:9">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A140" s="7">
         <v>6090</v>
       </c>
@@ -5225,7 +5230,7 @@
       <c r="H140" s="7"/>
       <c r="I140" s="7"/>
     </row>
-    <row r="141" spans="1:9">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A141" s="7">
         <v>6091</v>
       </c>
@@ -5248,7 +5253,7 @@
       <c r="H141" s="7"/>
       <c r="I141" s="7"/>
     </row>
-    <row r="142" spans="1:9">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A142" s="7">
         <v>6092</v>
       </c>
@@ -5271,7 +5276,7 @@
       <c r="H142" s="7"/>
       <c r="I142" s="7"/>
     </row>
-    <row r="143" spans="1:9">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A143" s="7">
         <v>6093</v>
       </c>
@@ -5294,7 +5299,7 @@
       <c r="H143" s="7"/>
       <c r="I143" s="7"/>
     </row>
-    <row r="144" spans="1:9">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A144" s="7">
         <v>6094</v>
       </c>
@@ -5317,7 +5322,7 @@
       <c r="H144" s="7"/>
       <c r="I144" s="7"/>
     </row>
-    <row r="145" spans="1:9">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A145" s="7">
         <v>6095</v>
       </c>
@@ -5340,7 +5345,7 @@
       <c r="H145" s="7"/>
       <c r="I145" s="7"/>
     </row>
-    <row r="146" spans="1:9">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A146" s="7">
         <v>6096</v>
       </c>
@@ -5363,7 +5368,7 @@
       <c r="H146" s="7"/>
       <c r="I146" s="7"/>
     </row>
-    <row r="147" spans="1:9">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A147" s="6">
         <v>6097</v>
       </c>
@@ -5384,7 +5389,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="148" spans="1:9">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A148" s="7">
         <v>6098</v>
       </c>
@@ -5407,7 +5412,7 @@
       <c r="H148" s="7"/>
       <c r="I148" s="7"/>
     </row>
-    <row r="149" spans="1:9">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A149" s="7">
         <v>6099</v>
       </c>
@@ -5430,7 +5435,7 @@
       <c r="H149" s="7"/>
       <c r="I149" s="7"/>
     </row>
-    <row r="150" spans="1:9">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A150" s="7">
         <v>6100</v>
       </c>
@@ -5453,7 +5458,7 @@
       <c r="H150" s="7"/>
       <c r="I150" s="7"/>
     </row>
-    <row r="151" spans="1:9">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A151" s="7">
         <v>6101</v>
       </c>
@@ -5476,7 +5481,7 @@
       <c r="H151" s="7"/>
       <c r="I151" s="7"/>
     </row>
-    <row r="152" spans="1:9">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A152" s="7">
         <v>6102</v>
       </c>
@@ -5499,7 +5504,7 @@
       <c r="H152" s="7"/>
       <c r="I152" s="7"/>
     </row>
-    <row r="153" spans="1:9">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A153" s="7">
         <v>6103</v>
       </c>
@@ -5522,7 +5527,7 @@
       <c r="H153" s="7"/>
       <c r="I153" s="7"/>
     </row>
-    <row r="154" spans="1:9">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A154" s="7">
         <v>6104</v>
       </c>
@@ -5545,7 +5550,7 @@
       <c r="H154" s="7"/>
       <c r="I154" s="7"/>
     </row>
-    <row r="155" spans="1:9">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A155" s="7">
         <v>6105</v>
       </c>
@@ -5568,7 +5573,7 @@
       <c r="H155" s="7"/>
       <c r="I155" s="7"/>
     </row>
-    <row r="156" spans="1:9">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A156" s="7">
         <v>6106</v>
       </c>
@@ -5591,7 +5596,7 @@
       <c r="H156" s="7"/>
       <c r="I156" s="7"/>
     </row>
-    <row r="157" spans="1:9">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A157" s="7">
         <v>6107</v>
       </c>
@@ -5614,7 +5619,7 @@
       <c r="H157" s="7"/>
       <c r="I157" s="7"/>
     </row>
-    <row r="158" spans="1:9">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A158" s="7">
         <v>6108</v>
       </c>
@@ -5639,7 +5644,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="159" spans="1:9">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A159" s="8">
         <v>606500</v>
       </c>
@@ -5666,7 +5671,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="160" spans="1:9">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A160" s="8">
         <v>606510</v>
       </c>
@@ -5689,7 +5694,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="161" spans="1:9">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A161" s="8">
         <v>606511</v>
       </c>
@@ -5716,7 +5721,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="162" spans="1:9">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A162" s="8">
         <v>606512</v>
       </c>
@@ -5743,7 +5748,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="163" spans="1:9">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A163" s="8">
         <v>606513</v>
       </c>
@@ -5770,7 +5775,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="164" spans="1:9">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A164" s="8">
         <v>606514</v>
       </c>
@@ -5795,7 +5800,7 @@
       </c>
       <c r="I164" s="8"/>
     </row>
-    <row r="165" spans="1:9">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A165" s="8">
         <v>606520</v>
       </c>
@@ -5822,7 +5827,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="166" spans="1:9">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A166" s="8">
         <v>606530</v>
       </c>
@@ -5849,7 +5854,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="167" spans="1:9">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A167" s="8">
         <v>606531</v>
       </c>
@@ -5876,7 +5881,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="168" spans="1:9">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A168" s="8">
         <v>606532</v>
       </c>
@@ -5903,7 +5908,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="169" spans="1:9">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A169" s="8">
         <v>606533</v>
       </c>
@@ -5928,7 +5933,7 @@
       </c>
       <c r="I169" s="8"/>
     </row>
-    <row r="170" spans="1:9">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A170" s="8">
         <v>606540</v>
       </c>
@@ -5955,7 +5960,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="171" spans="1:9">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A171" s="8">
         <v>606541</v>
       </c>
@@ -5980,7 +5985,7 @@
       </c>
       <c r="I171" s="8"/>
     </row>
-    <row r="172" spans="1:9">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A172" s="8">
         <v>606542</v>
       </c>
@@ -6005,7 +6010,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="173" spans="1:9">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A173" s="8">
         <v>606550</v>
       </c>
@@ -6016,7 +6021,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="174" spans="1:9">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A174" s="8">
         <v>606551</v>
       </c>
@@ -6039,7 +6044,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="175" spans="1:9">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A175" s="8">
         <v>606552</v>
       </c>
@@ -6066,7 +6071,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="176" spans="1:9">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A176" s="10">
         <v>604300</v>
       </c>
@@ -6093,7 +6098,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="177" spans="1:9">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A177" s="8">
         <v>607100</v>
       </c>
@@ -6119,7 +6124,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="178" spans="1:9">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A178" s="8">
         <v>607110</v>
       </c>
@@ -6142,7 +6147,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="179" spans="1:9">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A179" s="8">
         <v>607120</v>
       </c>
@@ -6168,7 +6173,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="180" spans="1:9">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A180" s="8">
         <v>607130</v>
       </c>
@@ -6194,7 +6199,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="181" spans="1:9">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A181" s="8">
         <v>607140</v>
       </c>
@@ -6220,7 +6225,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="182" spans="1:9">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A182" s="8">
         <v>607150</v>
       </c>
@@ -6243,7 +6248,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="183" spans="1:9">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A183" s="8">
         <v>607160</v>
       </c>
@@ -6269,7 +6274,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="184" spans="1:9">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A184" s="8">
         <v>607170</v>
       </c>
@@ -6295,7 +6300,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="185" spans="1:9">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A185" s="8">
         <v>607180</v>
       </c>
@@ -6312,7 +6317,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="186" spans="1:9">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A186" s="8">
         <v>607190</v>
       </c>
@@ -6335,7 +6340,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="187" spans="1:9">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A187" s="8">
         <v>607200</v>
       </c>
@@ -6361,7 +6366,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="188" spans="1:9">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A188" s="8">
         <v>607210</v>
       </c>
@@ -6378,7 +6383,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="189" spans="1:9">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A189" s="8">
         <v>607220</v>
       </c>
@@ -6404,7 +6409,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="190" spans="1:9" ht="15" customHeight="1">
+    <row r="190" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190" s="8">
         <v>607230</v>
       </c>
@@ -6427,7 +6432,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="191" spans="1:9">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A191" s="8">
         <v>603600</v>
       </c>
@@ -6453,7 +6458,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="192" spans="1:9">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A192" s="8">
         <v>603610</v>
       </c>
@@ -6482,7 +6487,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="193" spans="1:9">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A193" s="8">
         <v>600200</v>
       </c>
@@ -6508,7 +6513,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="194" spans="1:9">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A194" s="8">
         <v>600210</v>
       </c>
@@ -6535,7 +6540,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="195" spans="1:9">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A195" s="8">
         <v>600220</v>
       </c>
@@ -6561,7 +6566,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="196" spans="1:9">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A196" s="8">
         <v>600230</v>
       </c>
@@ -6587,7 +6592,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="197" spans="1:9">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A197" s="8">
         <v>600240</v>
       </c>
@@ -6613,7 +6618,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="198" spans="1:9">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A198" s="8">
         <v>605600</v>
       </c>
@@ -6639,7 +6644,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="199" spans="1:9">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A199" s="8">
         <v>610800</v>
       </c>
@@ -6665,7 +6670,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="200" spans="1:9">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A200" s="8">
         <v>605300</v>
       </c>
@@ -6697,11 +6702,6 @@
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -6710,11 +6710,11 @@
   <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.33203125" customWidth="1"/>
     <col min="2" max="2" width="14.83203125" customWidth="1"/>
@@ -6722,7 +6722,7 @@
     <col min="5" max="5" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -6742,7 +6742,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -6762,7 +6762,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -6773,7 +6773,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -6793,7 +6793,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -6813,7 +6813,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -6833,7 +6833,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -6853,7 +6853,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -6873,7 +6873,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -6893,7 +6893,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -6915,10 +6915,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
removes double admin menu after menu load
</commit_message>
<xml_diff>
--- a/application/import_data/menus.xlsx
+++ b/application/import_data/menus.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="2960" windowWidth="24860" windowHeight="14560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="740" yWindow="1440" windowWidth="24860" windowHeight="14560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="menus" sheetId="2" r:id="rId1"/>
@@ -1976,11 +1976,14 @@
   <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:I180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="117" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="16.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">

</xml_diff>

<commit_message>
fixes page head and includes updated menus excel file
</commit_message>
<xml_diff>
--- a/application/import_data/menus.xlsx
+++ b/application/import_data/menus.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mneucollins/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mneucollins/Sites/PhpstormProjects/PWM/resources/csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1051,13 +1051,13 @@
     <t>Our Partners</t>
   </si>
   <si>
-    <t>Telling the Weather…</t>
-  </si>
-  <si>
     <t>Null</t>
   </si>
   <si>
     <t>[base_url]/index.php/mainmenu/gottschalk_book</t>
+  </si>
+  <si>
+    <t>Predicting the Weather…</t>
   </si>
 </sst>
 </file>
@@ -1980,7 +1980,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2177,13 +2177,13 @@
         <v>3</v>
       </c>
       <c r="E7" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="G7" s="5" t="s">
         <v>310</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>311</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
adds new counties to the menus
</commit_message>
<xml_diff>
--- a/application/import_data/menus.xlsx
+++ b/application/import_data/menus.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4580" yWindow="660" windowWidth="18580" windowHeight="14260" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="660" yWindow="460" windowWidth="24940" windowHeight="15540" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="menus" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1534" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1577" uniqueCount="328">
   <si>
     <t>secondary_menu</t>
   </si>
@@ -1012,9 +1012,6 @@
     <t>[base_url]/index.php/home/view/cedar/6071</t>
   </si>
   <si>
-    <t>[base_url]/index.php/home/view/lee//6108</t>
-  </si>
-  <si>
     <t>[base_url]/index.php/home/story/6053</t>
   </si>
   <si>
@@ -1058,13 +1055,64 @@
   </si>
   <si>
     <t>Predicting the Weather…</t>
+  </si>
+  <si>
+    <t>[base_url]/index.php/mainmenu/about/1</t>
+  </si>
+  <si>
+    <t>[base_url]/index.php/mainmenu/about/0</t>
+  </si>
+  <si>
+    <t>[base_url]/index.php/mainmenu/about/2</t>
+  </si>
+  <si>
+    <t>[base_url]/index.php/mainmenu/about/3</t>
+  </si>
+  <si>
+    <t>[base_url]/index.php/home/view/lee/6108</t>
+  </si>
+  <si>
+    <t>[base_url]/index.php/home/view/blackhawk/6059</t>
+  </si>
+  <si>
+    <t>[base_url]/index.php/home/view/boone/6052</t>
+  </si>
+  <si>
+    <t>[base_url]/index.php/home/view/scott/6074</t>
+  </si>
+  <si>
+    <t>[base_url]/index.php/home/view/wapello/6102</t>
+  </si>
+  <si>
+    <t>Blackhawk County</t>
+  </si>
+  <si>
+    <t>Boone County</t>
+  </si>
+  <si>
+    <t>Scott County</t>
+  </si>
+  <si>
+    <t>Wapello County</t>
+  </si>
+  <si>
+    <t>blackhawk</t>
+  </si>
+  <si>
+    <t>boone</t>
+  </si>
+  <si>
+    <t>scott</t>
+  </si>
+  <si>
+    <t>wapello</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1101,8 +1149,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1143,6 +1196,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD8E4BC"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1276,7 +1335,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -1304,6 +1363,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1761,10 +1824,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1964,6 +2028,74 @@
         <v>13</v>
       </c>
     </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A12" s="1">
+        <v>6059</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A13" s="1">
+        <v>6052</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A14" s="1">
+        <v>6074</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A15" s="1">
+        <v>6102</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1977,16 +2109,18 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:I175"/>
+  <dimension ref="A1:I179"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A159" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F177" sqref="F177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="5" max="5" width="27.5" customWidth="1"/>
     <col min="6" max="6" width="16.33203125" customWidth="1"/>
-    <col min="7" max="7" width="38" customWidth="1"/>
+    <col min="7" max="7" width="51.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -2061,7 +2195,7 @@
         <v>280</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>280</v>
@@ -2177,13 +2311,13 @@
         <v>3</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F7" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>309</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>310</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>12</v>
@@ -2424,7 +2558,7 @@
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
@@ -2443,7 +2577,7 @@
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
@@ -2462,7 +2596,7 @@
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
@@ -2518,7 +2652,7 @@
         <v>280</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>13</v>
+        <v>312</v>
       </c>
       <c r="H20" s="5" t="s">
         <v>12</v>
@@ -2539,10 +2673,12 @@
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
+      <c r="G21" s="5" t="s">
+        <v>311</v>
+      </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
     </row>
@@ -2558,10 +2694,12 @@
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
+      <c r="G22" s="5" t="s">
+        <v>313</v>
+      </c>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
     </row>
@@ -2577,10 +2715,12 @@
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
+      <c r="G23" s="5" t="s">
+        <v>314</v>
+      </c>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
     </row>
@@ -2598,13 +2738,13 @@
         <v>280</v>
       </c>
       <c r="E24" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="G24" s="5" t="s">
         <v>300</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>301</v>
       </c>
       <c r="H24" s="5" t="s">
         <v>20</v>
@@ -4141,13 +4281,13 @@
         <v>280</v>
       </c>
       <c r="G77" t="s">
-        <v>13</v>
+        <v>317</v>
       </c>
       <c r="H77" t="s">
         <v>280</v>
       </c>
       <c r="I77" t="s">
-        <v>280</v>
+        <v>19</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
@@ -4344,13 +4484,13 @@
         <v>280</v>
       </c>
       <c r="G84" t="s">
-        <v>13</v>
+        <v>316</v>
       </c>
       <c r="H84" t="s">
         <v>280</v>
       </c>
       <c r="I84" t="s">
-        <v>280</v>
+        <v>19</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
@@ -4779,13 +4919,13 @@
         <v>280</v>
       </c>
       <c r="G99" t="s">
-        <v>13</v>
+        <v>318</v>
       </c>
       <c r="H99" t="s">
         <v>280</v>
       </c>
       <c r="I99" t="s">
-        <v>280</v>
+        <v>19</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
@@ -5591,13 +5731,13 @@
         <v>280</v>
       </c>
       <c r="G127" t="s">
-        <v>13</v>
+        <v>319</v>
       </c>
       <c r="H127" t="s">
         <v>280</v>
       </c>
       <c r="I127" t="s">
-        <v>280</v>
+        <v>19</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.2">
@@ -5765,7 +5905,7 @@
         <v>280</v>
       </c>
       <c r="G133" t="s">
-        <v>296</v>
+        <v>315</v>
       </c>
       <c r="H133" t="s">
         <v>280</v>
@@ -5775,31 +5915,31 @@
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A134" s="7">
+      <c r="A134" s="14">
         <v>600200</v>
       </c>
-      <c r="B134" s="7">
+      <c r="B134" s="14">
         <v>6002</v>
       </c>
-      <c r="C134" s="7" t="s">
-        <v>280</v>
-      </c>
-      <c r="D134" s="7">
+      <c r="C134" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="D134" s="14">
         <v>1</v>
       </c>
-      <c r="E134" s="7" t="s">
+      <c r="E134" s="14" t="s">
         <v>256</v>
       </c>
-      <c r="F134" s="7" t="s">
+      <c r="F134" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="G134" s="7" t="s">
+      <c r="G134" s="14" t="s">
         <v>258</v>
       </c>
-      <c r="H134" s="7" t="s">
+      <c r="H134" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I134" s="7" t="s">
+      <c r="I134" s="14" t="s">
         <v>212</v>
       </c>
     </row>
@@ -5920,31 +6060,31 @@
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A139" s="7">
+      <c r="A139" s="14">
         <v>603600</v>
       </c>
-      <c r="B139" s="7">
+      <c r="B139" s="14">
         <v>6036</v>
       </c>
-      <c r="C139" s="7" t="s">
-        <v>280</v>
-      </c>
-      <c r="D139" s="7">
+      <c r="C139" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="D139" s="14">
         <v>1</v>
       </c>
-      <c r="E139" s="7" t="s">
+      <c r="E139" s="14" t="s">
         <v>250</v>
       </c>
-      <c r="F139" s="7" t="s">
+      <c r="F139" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="G139" s="7" t="s">
+      <c r="G139" s="14" t="s">
         <v>254</v>
       </c>
-      <c r="H139" s="7" t="s">
+      <c r="H139" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I139" s="7" t="s">
+      <c r="I139" s="14" t="s">
         <v>212</v>
       </c>
     </row>
@@ -5978,118 +6118,118 @@
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A141" s="7">
+      <c r="A141" s="14">
         <v>604300</v>
       </c>
-      <c r="B141" s="7">
+      <c r="B141" s="14">
         <v>6043</v>
       </c>
-      <c r="C141" s="7" t="s">
-        <v>280</v>
-      </c>
-      <c r="D141" s="7">
+      <c r="C141" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="D141" s="14">
         <v>1</v>
       </c>
-      <c r="E141" s="7" t="s">
+      <c r="E141" s="14" t="s">
         <v>215</v>
       </c>
-      <c r="F141" s="7" t="s">
+      <c r="F141" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="G141" s="7" t="s">
+      <c r="G141" s="14" t="s">
         <v>291</v>
       </c>
-      <c r="H141" s="7" t="s">
+      <c r="H141" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I141" s="7" t="s">
+      <c r="I141" s="14" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A142" s="7">
+      <c r="A142" s="14">
         <v>605300</v>
       </c>
-      <c r="B142" s="7">
+      <c r="B142" s="14">
         <v>6053</v>
       </c>
-      <c r="C142" s="7" t="s">
-        <v>280</v>
-      </c>
-      <c r="D142" s="7">
+      <c r="C142" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="D142" s="14">
         <v>1</v>
       </c>
-      <c r="E142" s="7" t="s">
+      <c r="E142" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="F142" s="7" t="s">
+      <c r="F142" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="G142" s="7" t="s">
-        <v>297</v>
-      </c>
-      <c r="H142" s="7" t="s">
+      <c r="G142" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="H142" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I142" s="7" t="s">
+      <c r="I142" s="14" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A143" s="7">
+      <c r="A143" s="14">
         <v>605600</v>
       </c>
-      <c r="B143" s="7">
+      <c r="B143" s="14">
         <v>6056</v>
       </c>
-      <c r="C143" s="7" t="s">
-        <v>280</v>
-      </c>
-      <c r="D143" s="7">
+      <c r="C143" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="D143" s="14">
         <v>1</v>
       </c>
-      <c r="E143" s="7" t="s">
+      <c r="E143" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="F143" s="7" t="s">
+      <c r="F143" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="G143" s="7" t="s">
+      <c r="G143" s="14" t="s">
         <v>293</v>
       </c>
-      <c r="H143" s="7" t="s">
+      <c r="H143" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I143" s="7" t="s">
+      <c r="I143" s="14" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A144" s="7">
+      <c r="A144" s="14">
         <v>606500</v>
       </c>
-      <c r="B144" s="7">
+      <c r="B144" s="14">
         <v>6065</v>
       </c>
-      <c r="C144" s="7" t="s">
-        <v>280</v>
-      </c>
-      <c r="D144" s="7">
+      <c r="C144" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="D144" s="14">
         <v>1</v>
       </c>
-      <c r="E144" s="7" t="s">
+      <c r="E144" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="F144" s="7" t="s">
+      <c r="F144" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="G144" s="7" t="s">
+      <c r="G144" s="14" t="s">
         <v>294</v>
       </c>
-      <c r="H144" s="7" t="s">
+      <c r="H144" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I144" s="7" t="s">
+      <c r="I144" s="14" t="s">
         <v>212</v>
       </c>
     </row>
@@ -6142,7 +6282,7 @@
         <v>280</v>
       </c>
       <c r="G146" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H146" s="7" t="s">
         <v>12</v>
@@ -6426,7 +6566,7 @@
         <v>1</v>
       </c>
       <c r="E156" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F156" s="7" t="s">
         <v>280</v>
@@ -6558,31 +6698,31 @@
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A161" s="7">
+      <c r="A161" s="14">
         <v>607100</v>
       </c>
-      <c r="B161" s="7">
+      <c r="B161" s="14">
         <v>6071</v>
       </c>
-      <c r="C161" s="7" t="s">
-        <v>280</v>
-      </c>
-      <c r="D161" s="7">
+      <c r="C161" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="D161" s="14">
         <v>1</v>
       </c>
-      <c r="E161" s="7" t="s">
+      <c r="E161" s="14" t="s">
         <v>219</v>
       </c>
-      <c r="F161" s="7" t="s">
+      <c r="F161" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="G161" s="7" t="s">
+      <c r="G161" s="14" t="s">
         <v>295</v>
       </c>
-      <c r="H161" s="7" t="s">
+      <c r="H161" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I161" s="7" t="s">
+      <c r="I161" s="14" t="s">
         <v>212</v>
       </c>
     </row>
@@ -6964,46 +7104,164 @@
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A175" s="7">
+      <c r="A175" s="14">
         <v>610800</v>
       </c>
-      <c r="B175" s="7">
+      <c r="B175" s="14">
         <v>6108</v>
       </c>
-      <c r="C175" s="7" t="s">
-        <v>280</v>
-      </c>
-      <c r="D175" s="7">
+      <c r="C175" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="D175" s="14">
         <v>1</v>
       </c>
-      <c r="E175" s="7" t="s">
+      <c r="E175" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="F175" s="7" t="s">
+      <c r="F175" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="G175" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="H175" s="7" t="s">
+      <c r="G175" s="14" t="s">
+        <v>315</v>
+      </c>
+      <c r="H175" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I175" s="7" t="s">
+      <c r="I175" s="14" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A176" s="14">
+        <v>605900</v>
+      </c>
+      <c r="B176" s="14">
+        <v>6059</v>
+      </c>
+      <c r="C176" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="D176" s="14">
+        <v>1</v>
+      </c>
+      <c r="E176" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="F176" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="G176" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="H176" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="I176" s="14" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A177" s="14">
+        <v>605200</v>
+      </c>
+      <c r="B177" s="14">
+        <v>6052</v>
+      </c>
+      <c r="C177" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="D177" s="14">
+        <v>1</v>
+      </c>
+      <c r="E177" s="14" t="s">
+        <v>321</v>
+      </c>
+      <c r="F177" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="G177" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="H177" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="I177" s="14" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A178" s="14">
+        <v>607400</v>
+      </c>
+      <c r="B178" s="14">
+        <v>6074</v>
+      </c>
+      <c r="C178" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="D178" s="14">
+        <v>1</v>
+      </c>
+      <c r="E178" s="14" t="s">
+        <v>322</v>
+      </c>
+      <c r="F178" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="G178" s="14" t="s">
+        <v>318</v>
+      </c>
+      <c r="H178" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="I178" s="14" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A179" s="14">
+        <v>610200</v>
+      </c>
+      <c r="B179" s="14">
+        <v>6102</v>
+      </c>
+      <c r="C179" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="D179" s="14">
+        <v>1</v>
+      </c>
+      <c r="E179" s="14" t="s">
+        <v>323</v>
+      </c>
+      <c r="F179" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="G179" s="14" t="s">
+        <v>319</v>
+      </c>
+      <c r="H179" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="I179" s="14" t="s">
         <v>212</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7014,7 +7272,7 @@
     <col min="5" max="5" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -7034,7 +7292,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7054,7 +7312,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -7065,7 +7323,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -7085,7 +7343,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -7105,7 +7363,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -7125,7 +7383,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -7145,7 +7403,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -7165,7 +7423,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -7185,7 +7443,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -7204,6 +7462,95 @@
       <c r="F10">
         <v>11</v>
       </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>6059</v>
+      </c>
+      <c r="C11" t="s">
+        <v>324</v>
+      </c>
+      <c r="D11">
+        <v>42.4978711247633</v>
+      </c>
+      <c r="E11">
+        <v>-92.332237232476402</v>
+      </c>
+      <c r="F11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>6052</v>
+      </c>
+      <c r="C12" t="s">
+        <v>325</v>
+      </c>
+      <c r="D12">
+        <v>42.061477636654303</v>
+      </c>
+      <c r="E12">
+        <v>-93.904655445367098</v>
+      </c>
+      <c r="F12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>6074</v>
+      </c>
+      <c r="C13" t="s">
+        <v>326</v>
+      </c>
+      <c r="D13">
+        <v>41.642079647891599</v>
+      </c>
+      <c r="E13">
+        <v>-90.6135635264217</v>
+      </c>
+      <c r="F13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>6102</v>
+      </c>
+      <c r="C14" t="s">
+        <v>327</v>
+      </c>
+      <c r="D14" s="13">
+        <v>41.018070100000003</v>
+      </c>
+      <c r="E14">
+        <v>-92.415463099999997</v>
+      </c>
+      <c r="F14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D15" s="13"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H16" s="13"/>
+    </row>
+    <row r="17" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H17" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7216,7 +7563,7 @@
   <dimension ref="A1:I200"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M160" sqref="M160"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
lots of things added and quickflip moved to template
</commit_message>
<xml_diff>
--- a/application/import_data/menus.xlsx
+++ b/application/import_data/menus.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="660" yWindow="460" windowWidth="24940" windowHeight="15540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="660" yWindow="460" windowWidth="24940" windowHeight="15540" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="menus" sheetId="2" r:id="rId1"/>
@@ -2204,9 +2204,9 @@
   <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:I198"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9:XFD9"/>
+    <sheetView zoomScale="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7855,9 +7855,9 @@
   <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView zoomScale="137" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7930,10 +7930,10 @@
         <v>217</v>
       </c>
       <c r="D4">
-        <v>41.723668064585503</v>
+        <v>41.684194446913601</v>
       </c>
       <c r="E4">
-        <v>-95.842666625976506</v>
+        <v>-95.766448974609304</v>
       </c>
       <c r="F4">
         <v>10</v>

</xml_diff>

<commit_message>
adds locally added images
</commit_message>
<xml_diff>
--- a/application/import_data/menus.xlsx
+++ b/application/import_data/menus.xlsx
@@ -2038,7 +2038,7 @@
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2445,11 +2445,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:I188"/>
+  <dimension ref="A1:I187"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+      <pane ySplit="1" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A165" sqref="A165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4051,37 +4051,37 @@
       <c r="I59" s="5"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A60" s="5">
-        <v>5130</v>
-      </c>
-      <c r="B60" s="5">
-        <v>100</v>
-      </c>
-      <c r="C60" s="5">
-        <v>5000</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>298</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="G60" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="H60" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I60" s="5" t="s">
-        <v>208</v>
+      <c r="A60" s="6">
+        <v>6000</v>
+      </c>
+      <c r="B60" s="6">
+        <v>200</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="G60" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H60" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="I60" s="6" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="6">
-        <v>6000</v>
+        <v>6001</v>
       </c>
       <c r="B61" s="6">
         <v>200</v>
@@ -4093,7 +4093,7 @@
         <v>280</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F61" s="6" t="s">
         <v>280</v>
@@ -4105,41 +4105,41 @@
         <v>280</v>
       </c>
       <c r="I61" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A62" s="6">
+      <c r="A62">
+        <v>6002</v>
+      </c>
+      <c r="B62">
+        <v>200</v>
+      </c>
+      <c r="C62">
         <v>6001</v>
       </c>
-      <c r="B62" s="6">
-        <v>200</v>
-      </c>
-      <c r="C62" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="D62" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="E62" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="F62" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G62" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H62" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I62" s="6" t="s">
-        <v>208</v>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62" t="s">
+        <v>147</v>
+      </c>
+      <c r="F62" t="s">
+        <v>280</v>
+      </c>
+      <c r="G62" t="s">
+        <v>258</v>
+      </c>
+      <c r="H62" t="s">
+        <v>280</v>
+      </c>
+      <c r="I62" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>6002</v>
+        <v>6003</v>
       </c>
       <c r="B63">
         <v>200</v>
@@ -4148,27 +4148,27 @@
         <v>6001</v>
       </c>
       <c r="D63">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E63" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="F63" t="s">
         <v>280</v>
       </c>
       <c r="G63" t="s">
-        <v>258</v>
+        <v>13</v>
       </c>
       <c r="H63" t="s">
         <v>280</v>
       </c>
       <c r="I63" t="s">
-        <v>19</v>
+        <v>280</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>6003</v>
+        <v>6004</v>
       </c>
       <c r="B64">
         <v>200</v>
@@ -4177,10 +4177,10 @@
         <v>6001</v>
       </c>
       <c r="D64">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E64" t="s">
-        <v>159</v>
+        <v>118</v>
       </c>
       <c r="F64" t="s">
         <v>280</v>
@@ -4197,7 +4197,7 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>6004</v>
+        <v>6005</v>
       </c>
       <c r="B65">
         <v>200</v>
@@ -4206,10 +4206,10 @@
         <v>6001</v>
       </c>
       <c r="D65">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E65" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F65" t="s">
         <v>280</v>
@@ -4226,7 +4226,7 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>6005</v>
+        <v>6006</v>
       </c>
       <c r="B66">
         <v>200</v>
@@ -4235,10 +4235,10 @@
         <v>6001</v>
       </c>
       <c r="D66">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E66" t="s">
-        <v>120</v>
+        <v>169</v>
       </c>
       <c r="F66" t="s">
         <v>280</v>
@@ -4255,7 +4255,7 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>6006</v>
+        <v>6007</v>
       </c>
       <c r="B67">
         <v>200</v>
@@ -4264,10 +4264,10 @@
         <v>6001</v>
       </c>
       <c r="D67">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E67" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="F67" t="s">
         <v>280</v>
@@ -4284,7 +4284,7 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>6007</v>
+        <v>6008</v>
       </c>
       <c r="B68">
         <v>200</v>
@@ -4293,27 +4293,27 @@
         <v>6001</v>
       </c>
       <c r="D68">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E68" t="s">
-        <v>158</v>
+        <v>109</v>
       </c>
       <c r="F68" t="s">
         <v>280</v>
       </c>
       <c r="G68" t="s">
-        <v>13</v>
+        <v>377</v>
       </c>
       <c r="H68" t="s">
         <v>280</v>
       </c>
       <c r="I68" t="s">
-        <v>280</v>
+        <v>19</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>6008</v>
+        <v>6009</v>
       </c>
       <c r="B69">
         <v>200</v>
@@ -4322,27 +4322,27 @@
         <v>6001</v>
       </c>
       <c r="D69">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E69" t="s">
-        <v>109</v>
+        <v>161</v>
       </c>
       <c r="F69" t="s">
         <v>280</v>
       </c>
       <c r="G69" t="s">
-        <v>377</v>
+        <v>13</v>
       </c>
       <c r="H69" t="s">
         <v>280</v>
       </c>
       <c r="I69" t="s">
-        <v>19</v>
+        <v>280</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>6009</v>
+        <v>6010</v>
       </c>
       <c r="B70">
         <v>200</v>
@@ -4351,10 +4351,10 @@
         <v>6001</v>
       </c>
       <c r="D70">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E70" t="s">
-        <v>161</v>
+        <v>187</v>
       </c>
       <c r="F70" t="s">
         <v>280</v>
@@ -4371,7 +4371,7 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>6010</v>
+        <v>6011</v>
       </c>
       <c r="B71">
         <v>200</v>
@@ -4380,10 +4380,10 @@
         <v>6001</v>
       </c>
       <c r="D71">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E71" t="s">
-        <v>187</v>
+        <v>106</v>
       </c>
       <c r="F71" t="s">
         <v>280</v>
@@ -4400,7 +4400,7 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>6011</v>
+        <v>6012</v>
       </c>
       <c r="B72">
         <v>200</v>
@@ -4409,10 +4409,10 @@
         <v>6001</v>
       </c>
       <c r="D72">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E72" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="F72" t="s">
         <v>280</v>
@@ -4429,7 +4429,7 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>6012</v>
+        <v>6013</v>
       </c>
       <c r="B73">
         <v>200</v>
@@ -4438,10 +4438,10 @@
         <v>6001</v>
       </c>
       <c r="D73">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E73" t="s">
-        <v>99</v>
+        <v>162</v>
       </c>
       <c r="F73" t="s">
         <v>280</v>
@@ -4457,66 +4457,66 @@
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A74">
-        <v>6013</v>
-      </c>
-      <c r="B74">
-        <v>200</v>
-      </c>
-      <c r="C74">
-        <v>6001</v>
-      </c>
-      <c r="D74">
-        <v>12</v>
-      </c>
-      <c r="E74" t="s">
-        <v>162</v>
-      </c>
-      <c r="F74" t="s">
-        <v>280</v>
-      </c>
-      <c r="G74" t="s">
-        <v>13</v>
-      </c>
-      <c r="H74" t="s">
-        <v>280</v>
-      </c>
-      <c r="I74" t="s">
-        <v>280</v>
+      <c r="A74" s="6">
+        <v>6014</v>
+      </c>
+      <c r="B74" s="6">
+        <v>200</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="E74" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="F74" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="G74" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H74" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="I74" s="6" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A75" s="6">
+      <c r="A75">
+        <v>6015</v>
+      </c>
+      <c r="B75">
+        <v>200</v>
+      </c>
+      <c r="C75">
         <v>6014</v>
       </c>
-      <c r="B75" s="6">
-        <v>200</v>
-      </c>
-      <c r="C75" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="D75" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="E75" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="F75" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G75" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H75" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I75" s="6" t="s">
-        <v>208</v>
+      <c r="D75">
+        <v>1</v>
+      </c>
+      <c r="E75" t="s">
+        <v>142</v>
+      </c>
+      <c r="F75" t="s">
+        <v>280</v>
+      </c>
+      <c r="G75" t="s">
+        <v>13</v>
+      </c>
+      <c r="H75" t="s">
+        <v>280</v>
+      </c>
+      <c r="I75" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>6015</v>
+        <v>6016</v>
       </c>
       <c r="B76">
         <v>200</v>
@@ -4525,10 +4525,10 @@
         <v>6014</v>
       </c>
       <c r="D76">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E76" t="s">
-        <v>142</v>
+        <v>180</v>
       </c>
       <c r="F76" t="s">
         <v>280</v>
@@ -4545,7 +4545,7 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>6016</v>
+        <v>6017</v>
       </c>
       <c r="B77">
         <v>200</v>
@@ -4554,10 +4554,10 @@
         <v>6014</v>
       </c>
       <c r="D77">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E77" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="F77" t="s">
         <v>280</v>
@@ -4574,7 +4574,7 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>6017</v>
+        <v>6018</v>
       </c>
       <c r="B78">
         <v>200</v>
@@ -4583,10 +4583,10 @@
         <v>6014</v>
       </c>
       <c r="D78">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E78" t="s">
-        <v>183</v>
+        <v>153</v>
       </c>
       <c r="F78" t="s">
         <v>280</v>
@@ -4603,7 +4603,7 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>6018</v>
+        <v>6019</v>
       </c>
       <c r="B79">
         <v>200</v>
@@ -4612,10 +4612,10 @@
         <v>6014</v>
       </c>
       <c r="D79">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E79" t="s">
-        <v>153</v>
+        <v>128</v>
       </c>
       <c r="F79" t="s">
         <v>280</v>
@@ -4632,7 +4632,7 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>6019</v>
+        <v>6020</v>
       </c>
       <c r="B80">
         <v>200</v>
@@ -4641,10 +4641,10 @@
         <v>6014</v>
       </c>
       <c r="D80">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E80" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="F80" t="s">
         <v>280</v>
@@ -4661,7 +4661,7 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>6020</v>
+        <v>6021</v>
       </c>
       <c r="B81">
         <v>200</v>
@@ -4670,10 +4670,10 @@
         <v>6014</v>
       </c>
       <c r="D81">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E81" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="F81" t="s">
         <v>280</v>
@@ -4690,7 +4690,7 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>6021</v>
+        <v>6022</v>
       </c>
       <c r="B82">
         <v>200</v>
@@ -4699,10 +4699,10 @@
         <v>6014</v>
       </c>
       <c r="D82">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E82" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="F82" t="s">
         <v>280</v>
@@ -4719,7 +4719,7 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>6022</v>
+        <v>6023</v>
       </c>
       <c r="B83">
         <v>200</v>
@@ -4728,10 +4728,10 @@
         <v>6014</v>
       </c>
       <c r="D83">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E83" t="s">
-        <v>133</v>
+        <v>184</v>
       </c>
       <c r="F83" t="s">
         <v>280</v>
@@ -4748,7 +4748,7 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>6023</v>
+        <v>6024</v>
       </c>
       <c r="B84">
         <v>200</v>
@@ -4757,10 +4757,10 @@
         <v>6014</v>
       </c>
       <c r="D84">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E84" t="s">
-        <v>184</v>
+        <v>123</v>
       </c>
       <c r="F84" t="s">
         <v>280</v>
@@ -4777,7 +4777,7 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85">
-        <v>6024</v>
+        <v>6025</v>
       </c>
       <c r="B85">
         <v>200</v>
@@ -4786,85 +4786,85 @@
         <v>6014</v>
       </c>
       <c r="D85">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E85" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="F85" t="s">
         <v>280</v>
       </c>
       <c r="G85" t="s">
-        <v>13</v>
+        <v>381</v>
       </c>
       <c r="H85" t="s">
         <v>280</v>
       </c>
       <c r="I85" t="s">
-        <v>280</v>
+        <v>19</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A86">
-        <v>6025</v>
-      </c>
-      <c r="B86">
-        <v>200</v>
-      </c>
-      <c r="C86">
-        <v>6014</v>
-      </c>
-      <c r="D86">
-        <v>11</v>
-      </c>
-      <c r="E86" t="s">
-        <v>100</v>
-      </c>
-      <c r="F86" t="s">
-        <v>280</v>
-      </c>
-      <c r="G86" t="s">
-        <v>381</v>
-      </c>
-      <c r="H86" t="s">
-        <v>280</v>
-      </c>
-      <c r="I86" t="s">
-        <v>19</v>
+      <c r="A86" s="6">
+        <v>6026</v>
+      </c>
+      <c r="B86" s="6">
+        <v>200</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="D86" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="E86" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F86" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="G86" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H86" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="I86" s="6" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A87" s="6">
+      <c r="A87">
+        <v>6027</v>
+      </c>
+      <c r="B87">
+        <v>200</v>
+      </c>
+      <c r="C87">
         <v>6026</v>
       </c>
-      <c r="B87" s="6">
-        <v>200</v>
-      </c>
-      <c r="C87" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="D87" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="E87" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="F87" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G87" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H87" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I87" s="6" t="s">
-        <v>208</v>
+      <c r="D87">
+        <v>1</v>
+      </c>
+      <c r="E87" t="s">
+        <v>132</v>
+      </c>
+      <c r="F87" t="s">
+        <v>280</v>
+      </c>
+      <c r="G87" t="s">
+        <v>13</v>
+      </c>
+      <c r="H87" t="s">
+        <v>280</v>
+      </c>
+      <c r="I87" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88">
-        <v>6027</v>
+        <v>6028</v>
       </c>
       <c r="B88">
         <v>200</v>
@@ -4873,10 +4873,10 @@
         <v>6026</v>
       </c>
       <c r="D88">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E88" t="s">
-        <v>132</v>
+        <v>181</v>
       </c>
       <c r="F88" t="s">
         <v>280</v>
@@ -4893,7 +4893,7 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89">
-        <v>6028</v>
+        <v>6029</v>
       </c>
       <c r="B89">
         <v>200</v>
@@ -4902,10 +4902,10 @@
         <v>6026</v>
       </c>
       <c r="D89">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E89" t="s">
-        <v>181</v>
+        <v>93</v>
       </c>
       <c r="F89" t="s">
         <v>280</v>
@@ -4922,7 +4922,7 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90">
-        <v>6029</v>
+        <v>6030</v>
       </c>
       <c r="B90">
         <v>200</v>
@@ -4931,10 +4931,10 @@
         <v>6026</v>
       </c>
       <c r="D90">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E90" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="F90" t="s">
         <v>280</v>
@@ -4951,7 +4951,7 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91">
-        <v>6030</v>
+        <v>6031</v>
       </c>
       <c r="B91">
         <v>200</v>
@@ -4960,10 +4960,10 @@
         <v>6026</v>
       </c>
       <c r="D91">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E91" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="F91" t="s">
         <v>280</v>
@@ -4980,7 +4980,7 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92">
-        <v>6031</v>
+        <v>6032</v>
       </c>
       <c r="B92">
         <v>200</v>
@@ -4989,10 +4989,10 @@
         <v>6026</v>
       </c>
       <c r="D92">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E92" t="s">
-        <v>97</v>
+        <v>121</v>
       </c>
       <c r="F92" t="s">
         <v>280</v>
@@ -5009,7 +5009,7 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93">
-        <v>6032</v>
+        <v>6033</v>
       </c>
       <c r="B93">
         <v>200</v>
@@ -5018,85 +5018,85 @@
         <v>6026</v>
       </c>
       <c r="D93">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E93" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F93" t="s">
         <v>280</v>
       </c>
       <c r="G93" t="s">
-        <v>13</v>
+        <v>380</v>
       </c>
       <c r="H93" t="s">
         <v>280</v>
       </c>
       <c r="I93" t="s">
-        <v>280</v>
+        <v>19</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A94">
-        <v>6033</v>
-      </c>
-      <c r="B94">
-        <v>200</v>
-      </c>
-      <c r="C94">
-        <v>6026</v>
-      </c>
-      <c r="D94">
-        <v>7</v>
-      </c>
-      <c r="E94" t="s">
-        <v>110</v>
-      </c>
-      <c r="F94" t="s">
-        <v>280</v>
-      </c>
-      <c r="G94" t="s">
-        <v>380</v>
-      </c>
-      <c r="H94" t="s">
-        <v>280</v>
-      </c>
-      <c r="I94" t="s">
-        <v>19</v>
+      <c r="A94" s="6">
+        <v>6034</v>
+      </c>
+      <c r="B94" s="6">
+        <v>200</v>
+      </c>
+      <c r="C94" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="D94" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="E94" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="F94" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="G94" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H94" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="I94" s="6" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A95" s="6">
+      <c r="A95">
+        <v>6035</v>
+      </c>
+      <c r="B95">
+        <v>200</v>
+      </c>
+      <c r="C95">
         <v>6034</v>
       </c>
-      <c r="B95" s="6">
-        <v>200</v>
-      </c>
-      <c r="C95" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="D95" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="E95" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="F95" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G95" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H95" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I95" s="6" t="s">
-        <v>208</v>
+      <c r="D95">
+        <v>1</v>
+      </c>
+      <c r="E95" t="s">
+        <v>182</v>
+      </c>
+      <c r="F95" t="s">
+        <v>280</v>
+      </c>
+      <c r="G95" t="s">
+        <v>13</v>
+      </c>
+      <c r="H95" t="s">
+        <v>280</v>
+      </c>
+      <c r="I95" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96">
-        <v>6035</v>
+        <v>6036</v>
       </c>
       <c r="B96">
         <v>200</v>
@@ -5105,27 +5105,27 @@
         <v>6034</v>
       </c>
       <c r="D96">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E96" t="s">
-        <v>182</v>
+        <v>134</v>
       </c>
       <c r="F96" t="s">
         <v>280</v>
       </c>
       <c r="G96" t="s">
-        <v>13</v>
+        <v>254</v>
       </c>
       <c r="H96" t="s">
         <v>280</v>
       </c>
       <c r="I96" t="s">
-        <v>280</v>
+        <v>19</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97">
-        <v>6036</v>
+        <v>6037</v>
       </c>
       <c r="B97">
         <v>200</v>
@@ -5134,27 +5134,27 @@
         <v>6034</v>
       </c>
       <c r="D97">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E97" t="s">
-        <v>134</v>
+        <v>166</v>
       </c>
       <c r="F97" t="s">
         <v>280</v>
       </c>
       <c r="G97" t="s">
-        <v>254</v>
+        <v>13</v>
       </c>
       <c r="H97" t="s">
         <v>280</v>
       </c>
       <c r="I97" t="s">
-        <v>19</v>
+        <v>280</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98">
-        <v>6037</v>
+        <v>6038</v>
       </c>
       <c r="B98">
         <v>200</v>
@@ -5163,10 +5163,10 @@
         <v>6034</v>
       </c>
       <c r="D98">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E98" t="s">
-        <v>166</v>
+        <v>101</v>
       </c>
       <c r="F98" t="s">
         <v>280</v>
@@ -5183,7 +5183,7 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99">
-        <v>6038</v>
+        <v>6039</v>
       </c>
       <c r="B99">
         <v>200</v>
@@ -5192,10 +5192,10 @@
         <v>6034</v>
       </c>
       <c r="D99">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E99" t="s">
-        <v>101</v>
+        <v>154</v>
       </c>
       <c r="F99" t="s">
         <v>280</v>
@@ -5212,7 +5212,7 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100">
-        <v>6039</v>
+        <v>6040</v>
       </c>
       <c r="B100">
         <v>200</v>
@@ -5221,10 +5221,10 @@
         <v>6034</v>
       </c>
       <c r="D100">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E100" t="s">
-        <v>154</v>
+        <v>112</v>
       </c>
       <c r="F100" t="s">
         <v>280</v>
@@ -5241,7 +5241,7 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101">
-        <v>6040</v>
+        <v>6041</v>
       </c>
       <c r="B101">
         <v>200</v>
@@ -5250,10 +5250,10 @@
         <v>6034</v>
       </c>
       <c r="D101">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E101" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="F101" t="s">
         <v>280</v>
@@ -5270,7 +5270,7 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102">
-        <v>6041</v>
+        <v>6042</v>
       </c>
       <c r="B102">
         <v>200</v>
@@ -5279,10 +5279,10 @@
         <v>6034</v>
       </c>
       <c r="D102">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E102" t="s">
-        <v>102</v>
+        <v>125</v>
       </c>
       <c r="F102" t="s">
         <v>280</v>
@@ -5299,7 +5299,7 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103">
-        <v>6042</v>
+        <v>6043</v>
       </c>
       <c r="B103">
         <v>200</v>
@@ -5308,27 +5308,27 @@
         <v>6034</v>
       </c>
       <c r="D103">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E103" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="F103" t="s">
         <v>280</v>
       </c>
       <c r="G103" t="s">
-        <v>13</v>
+        <v>291</v>
       </c>
       <c r="H103" t="s">
         <v>280</v>
       </c>
       <c r="I103" t="s">
-        <v>280</v>
+        <v>19</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104">
-        <v>6043</v>
+        <v>6044</v>
       </c>
       <c r="B104">
         <v>200</v>
@@ -5337,27 +5337,27 @@
         <v>6034</v>
       </c>
       <c r="D104">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E104" t="s">
-        <v>130</v>
+        <v>168</v>
       </c>
       <c r="F104" t="s">
         <v>280</v>
       </c>
       <c r="G104" t="s">
-        <v>291</v>
+        <v>13</v>
       </c>
       <c r="H104" t="s">
         <v>280</v>
       </c>
       <c r="I104" t="s">
-        <v>19</v>
+        <v>280</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105">
-        <v>6044</v>
+        <v>6045</v>
       </c>
       <c r="B105">
         <v>200</v>
@@ -5366,10 +5366,10 @@
         <v>6034</v>
       </c>
       <c r="D105">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E105" t="s">
-        <v>168</v>
+        <v>192</v>
       </c>
       <c r="F105" t="s">
         <v>280</v>
@@ -5386,7 +5386,7 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106">
-        <v>6045</v>
+        <v>6046</v>
       </c>
       <c r="B106">
         <v>200</v>
@@ -5395,10 +5395,10 @@
         <v>6034</v>
       </c>
       <c r="D106">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E106" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="F106" t="s">
         <v>280</v>
@@ -5414,66 +5414,66 @@
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A107">
-        <v>6046</v>
-      </c>
-      <c r="B107">
-        <v>200</v>
-      </c>
-      <c r="C107">
-        <v>6034</v>
-      </c>
-      <c r="D107">
-        <v>12</v>
-      </c>
-      <c r="E107" t="s">
-        <v>193</v>
-      </c>
-      <c r="F107" t="s">
-        <v>280</v>
-      </c>
-      <c r="G107" t="s">
-        <v>13</v>
-      </c>
-      <c r="H107" t="s">
-        <v>280</v>
-      </c>
-      <c r="I107" t="s">
-        <v>280</v>
+      <c r="A107" s="6">
+        <v>6047</v>
+      </c>
+      <c r="B107" s="6">
+        <v>200</v>
+      </c>
+      <c r="C107" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="D107" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="E107" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="F107" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="G107" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H107" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="I107" s="6" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A108" s="6">
+      <c r="A108">
+        <v>6048</v>
+      </c>
+      <c r="B108">
+        <v>200</v>
+      </c>
+      <c r="C108">
         <v>6047</v>
       </c>
-      <c r="B108" s="6">
-        <v>200</v>
-      </c>
-      <c r="C108" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="D108" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="E108" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="F108" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G108" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H108" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I108" s="6" t="s">
-        <v>208</v>
+      <c r="D108">
+        <v>1</v>
+      </c>
+      <c r="E108" t="s">
+        <v>179</v>
+      </c>
+      <c r="F108" t="s">
+        <v>280</v>
+      </c>
+      <c r="G108" t="s">
+        <v>13</v>
+      </c>
+      <c r="H108" t="s">
+        <v>280</v>
+      </c>
+      <c r="I108" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109">
-        <v>6048</v>
+        <v>6049</v>
       </c>
       <c r="B109">
         <v>200</v>
@@ -5482,10 +5482,10 @@
         <v>6047</v>
       </c>
       <c r="D109">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E109" t="s">
-        <v>179</v>
+        <v>127</v>
       </c>
       <c r="F109" t="s">
         <v>280</v>
@@ -5502,7 +5502,7 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110">
-        <v>6049</v>
+        <v>6050</v>
       </c>
       <c r="B110">
         <v>200</v>
@@ -5511,10 +5511,10 @@
         <v>6047</v>
       </c>
       <c r="D110">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E110" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F110" t="s">
         <v>280</v>
@@ -5531,7 +5531,7 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111">
-        <v>6050</v>
+        <v>6051</v>
       </c>
       <c r="B111">
         <v>200</v>
@@ -5540,10 +5540,10 @@
         <v>6047</v>
       </c>
       <c r="D111">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E111" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F111" t="s">
         <v>280</v>
@@ -5560,7 +5560,7 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112">
-        <v>6051</v>
+        <v>6052</v>
       </c>
       <c r="B112">
         <v>200</v>
@@ -5569,27 +5569,27 @@
         <v>6047</v>
       </c>
       <c r="D112">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E112" t="s">
-        <v>126</v>
+        <v>96</v>
       </c>
       <c r="F112" t="s">
         <v>280</v>
       </c>
       <c r="G112" t="s">
-        <v>13</v>
+        <v>313</v>
       </c>
       <c r="H112" t="s">
         <v>280</v>
       </c>
       <c r="I112" t="s">
-        <v>280</v>
+        <v>19</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113">
-        <v>6052</v>
+        <v>6053</v>
       </c>
       <c r="B113">
         <v>200</v>
@@ -5598,16 +5598,16 @@
         <v>6047</v>
       </c>
       <c r="D113">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E113" t="s">
-        <v>96</v>
+        <v>170</v>
       </c>
       <c r="F113" t="s">
         <v>280</v>
       </c>
       <c r="G113" t="s">
-        <v>313</v>
+        <v>292</v>
       </c>
       <c r="H113" t="s">
         <v>280</v>
@@ -5618,7 +5618,7 @@
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A114">
-        <v>6053</v>
+        <v>6054</v>
       </c>
       <c r="B114">
         <v>200</v>
@@ -5627,27 +5627,27 @@
         <v>6047</v>
       </c>
       <c r="D114">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E114" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="F114" t="s">
         <v>280</v>
       </c>
       <c r="G114" t="s">
-        <v>292</v>
+        <v>13</v>
       </c>
       <c r="H114" t="s">
         <v>280</v>
       </c>
       <c r="I114" t="s">
-        <v>19</v>
+        <v>280</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115">
-        <v>6054</v>
+        <v>6055</v>
       </c>
       <c r="B115">
         <v>200</v>
@@ -5656,10 +5656,10 @@
         <v>6047</v>
       </c>
       <c r="D115">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E115" t="s">
-        <v>151</v>
+        <v>113</v>
       </c>
       <c r="F115" t="s">
         <v>280</v>
@@ -5676,7 +5676,7 @@
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A116">
-        <v>6055</v>
+        <v>6056</v>
       </c>
       <c r="B116">
         <v>200</v>
@@ -5685,10 +5685,10 @@
         <v>6047</v>
       </c>
       <c r="D116">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E116" t="s">
-        <v>113</v>
+        <v>163</v>
       </c>
       <c r="F116" t="s">
         <v>280</v>
@@ -5705,7 +5705,7 @@
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A117">
-        <v>6056</v>
+        <v>6057</v>
       </c>
       <c r="B117">
         <v>200</v>
@@ -5714,10 +5714,10 @@
         <v>6047</v>
       </c>
       <c r="D117">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E117" t="s">
-        <v>163</v>
+        <v>137</v>
       </c>
       <c r="F117" t="s">
         <v>280</v>
@@ -5733,66 +5733,66 @@
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A118">
-        <v>6057</v>
-      </c>
-      <c r="B118">
-        <v>200</v>
-      </c>
-      <c r="C118">
-        <v>6047</v>
-      </c>
-      <c r="D118">
-        <v>10</v>
-      </c>
-      <c r="E118" t="s">
-        <v>137</v>
-      </c>
-      <c r="F118" t="s">
-        <v>280</v>
-      </c>
-      <c r="G118" t="s">
-        <v>13</v>
-      </c>
-      <c r="H118" t="s">
-        <v>280</v>
-      </c>
-      <c r="I118" t="s">
-        <v>280</v>
+      <c r="A118" s="6">
+        <v>6058</v>
+      </c>
+      <c r="B118" s="6">
+        <v>200</v>
+      </c>
+      <c r="C118" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="D118" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="E118" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="F118" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="G118" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H118" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="I118" s="6" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A119" s="6">
+      <c r="A119">
+        <v>6059</v>
+      </c>
+      <c r="B119">
+        <v>200</v>
+      </c>
+      <c r="C119">
         <v>6058</v>
       </c>
-      <c r="B119" s="6">
-        <v>200</v>
-      </c>
-      <c r="C119" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="D119" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="E119" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="F119" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G119" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H119" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I119" s="6" t="s">
-        <v>208</v>
+      <c r="D119">
+        <v>1</v>
+      </c>
+      <c r="E119" t="s">
+        <v>196</v>
+      </c>
+      <c r="F119" t="s">
+        <v>280</v>
+      </c>
+      <c r="G119" t="s">
+        <v>312</v>
+      </c>
+      <c r="H119" t="s">
+        <v>280</v>
+      </c>
+      <c r="I119" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A120">
-        <v>6059</v>
+        <v>6060</v>
       </c>
       <c r="B120">
         <v>200</v>
@@ -5801,27 +5801,27 @@
         <v>6058</v>
       </c>
       <c r="D120">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E120" t="s">
-        <v>196</v>
+        <v>98</v>
       </c>
       <c r="F120" t="s">
         <v>280</v>
       </c>
       <c r="G120" t="s">
-        <v>312</v>
+        <v>13</v>
       </c>
       <c r="H120" t="s">
         <v>280</v>
       </c>
       <c r="I120" t="s">
-        <v>19</v>
+        <v>280</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A121">
-        <v>6060</v>
+        <v>6061</v>
       </c>
       <c r="B121">
         <v>200</v>
@@ -5830,10 +5830,10 @@
         <v>6058</v>
       </c>
       <c r="D121">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E121" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
       <c r="F121" t="s">
         <v>280</v>
@@ -5850,7 +5850,7 @@
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A122">
-        <v>6061</v>
+        <v>6062</v>
       </c>
       <c r="B122">
         <v>200</v>
@@ -5859,10 +5859,10 @@
         <v>6058</v>
       </c>
       <c r="D122">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E122" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F122" t="s">
         <v>280</v>
@@ -5879,7 +5879,7 @@
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A123">
-        <v>6062</v>
+        <v>6063</v>
       </c>
       <c r="B123">
         <v>200</v>
@@ -5888,10 +5888,10 @@
         <v>6058</v>
       </c>
       <c r="D123">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E123" t="s">
-        <v>119</v>
+        <v>171</v>
       </c>
       <c r="F123" t="s">
         <v>280</v>
@@ -5908,7 +5908,7 @@
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A124">
-        <v>6063</v>
+        <v>6064</v>
       </c>
       <c r="B124">
         <v>200</v>
@@ -5917,10 +5917,10 @@
         <v>6058</v>
       </c>
       <c r="D124">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E124" t="s">
-        <v>171</v>
+        <v>95</v>
       </c>
       <c r="F124" t="s">
         <v>280</v>
@@ -5937,7 +5937,7 @@
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A125">
-        <v>6064</v>
+        <v>6065</v>
       </c>
       <c r="B125">
         <v>200</v>
@@ -5946,27 +5946,27 @@
         <v>6058</v>
       </c>
       <c r="D125">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E125" t="s">
-        <v>95</v>
+        <v>144</v>
       </c>
       <c r="F125" t="s">
         <v>280</v>
       </c>
       <c r="G125" t="s">
-        <v>13</v>
+        <v>294</v>
       </c>
       <c r="H125" t="s">
         <v>280</v>
       </c>
       <c r="I125" t="s">
-        <v>280</v>
+        <v>19</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A126">
-        <v>6065</v>
+        <v>6066</v>
       </c>
       <c r="B126">
         <v>200</v>
@@ -5975,27 +5975,27 @@
         <v>6058</v>
       </c>
       <c r="D126">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E126" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F126" t="s">
         <v>280</v>
       </c>
       <c r="G126" t="s">
-        <v>294</v>
+        <v>13</v>
       </c>
       <c r="H126" t="s">
         <v>280</v>
       </c>
       <c r="I126" t="s">
-        <v>19</v>
+        <v>280</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A127">
-        <v>6066</v>
+        <v>6067</v>
       </c>
       <c r="B127">
         <v>200</v>
@@ -6004,10 +6004,10 @@
         <v>6058</v>
       </c>
       <c r="D127">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E127" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F127" t="s">
         <v>280</v>
@@ -6024,7 +6024,7 @@
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A128">
-        <v>6067</v>
+        <v>6068</v>
       </c>
       <c r="B128">
         <v>200</v>
@@ -6033,10 +6033,10 @@
         <v>6058</v>
       </c>
       <c r="D128">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E128" t="s">
-        <v>136</v>
+        <v>165</v>
       </c>
       <c r="F128" t="s">
         <v>280</v>
@@ -6053,7 +6053,7 @@
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A129">
-        <v>6068</v>
+        <v>6069</v>
       </c>
       <c r="B129">
         <v>200</v>
@@ -6062,10 +6062,10 @@
         <v>6058</v>
       </c>
       <c r="D129">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E129" t="s">
-        <v>165</v>
+        <v>135</v>
       </c>
       <c r="F129" t="s">
         <v>280</v>
@@ -6082,7 +6082,7 @@
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A130">
-        <v>6069</v>
+        <v>6070</v>
       </c>
       <c r="B130">
         <v>200</v>
@@ -6091,27 +6091,27 @@
         <v>6058</v>
       </c>
       <c r="D130">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E130" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="F130" t="s">
         <v>280</v>
       </c>
-      <c r="G130" t="s">
-        <v>13</v>
+      <c r="G130" s="14" t="s">
+        <v>386</v>
       </c>
       <c r="H130" t="s">
         <v>280</v>
       </c>
       <c r="I130" t="s">
-        <v>280</v>
+        <v>19</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A131">
-        <v>6070</v>
+        <v>6071</v>
       </c>
       <c r="B131">
         <v>200</v>
@@ -6120,16 +6120,16 @@
         <v>6058</v>
       </c>
       <c r="D131">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E131" t="s">
-        <v>139</v>
+        <v>104</v>
       </c>
       <c r="F131" t="s">
         <v>280</v>
       </c>
-      <c r="G131" s="14" t="s">
-        <v>386</v>
+      <c r="G131" t="s">
+        <v>295</v>
       </c>
       <c r="H131" t="s">
         <v>280</v>
@@ -6140,7 +6140,7 @@
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A132">
-        <v>6071</v>
+        <v>6072</v>
       </c>
       <c r="B132">
         <v>200</v>
@@ -6149,27 +6149,27 @@
         <v>6058</v>
       </c>
       <c r="D132">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E132" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="F132" t="s">
         <v>280</v>
       </c>
       <c r="G132" t="s">
-        <v>295</v>
+        <v>13</v>
       </c>
       <c r="H132" t="s">
         <v>280</v>
       </c>
       <c r="I132" t="s">
-        <v>19</v>
+        <v>280</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A133">
-        <v>6072</v>
+        <v>6073</v>
       </c>
       <c r="B133">
         <v>200</v>
@@ -6178,10 +6178,10 @@
         <v>6058</v>
       </c>
       <c r="D133">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E133" t="s">
-        <v>111</v>
+        <v>157</v>
       </c>
       <c r="F133" t="s">
         <v>280</v>
@@ -6198,7 +6198,7 @@
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A134">
-        <v>6073</v>
+        <v>6074</v>
       </c>
       <c r="B134">
         <v>200</v>
@@ -6207,85 +6207,85 @@
         <v>6058</v>
       </c>
       <c r="D134">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E134" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="F134" t="s">
         <v>280</v>
       </c>
       <c r="G134" t="s">
-        <v>13</v>
+        <v>314</v>
       </c>
       <c r="H134" t="s">
         <v>280</v>
       </c>
       <c r="I134" t="s">
-        <v>280</v>
+        <v>19</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A135">
-        <v>6074</v>
-      </c>
-      <c r="B135">
-        <v>200</v>
-      </c>
-      <c r="C135">
-        <v>6058</v>
-      </c>
-      <c r="D135">
-        <v>16</v>
-      </c>
-      <c r="E135" t="s">
-        <v>167</v>
-      </c>
-      <c r="F135" t="s">
-        <v>280</v>
-      </c>
-      <c r="G135" t="s">
-        <v>314</v>
-      </c>
-      <c r="H135" t="s">
-        <v>280</v>
-      </c>
-      <c r="I135" t="s">
+      <c r="A135" s="6">
+        <v>6075</v>
+      </c>
+      <c r="B135" s="6">
+        <v>200</v>
+      </c>
+      <c r="C135" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="D135" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="E135" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="F135" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="G135" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H135" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="I135" s="6" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>6076</v>
+      </c>
+      <c r="B136">
+        <v>200</v>
+      </c>
+      <c r="C136">
+        <v>6075</v>
+      </c>
+      <c r="D136">
+        <v>1</v>
+      </c>
+      <c r="E136" t="s">
+        <v>164</v>
+      </c>
+      <c r="F136" t="s">
+        <v>280</v>
+      </c>
+      <c r="G136" t="s">
+        <v>371</v>
+      </c>
+      <c r="H136" t="s">
+        <v>280</v>
+      </c>
+      <c r="I136" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A136" s="6">
-        <v>6075</v>
-      </c>
-      <c r="B136" s="6">
-        <v>200</v>
-      </c>
-      <c r="C136" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="D136" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="E136" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="F136" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G136" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H136" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I136" s="6" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A137">
-        <v>6076</v>
+        <v>6077</v>
       </c>
       <c r="B137">
         <v>200</v>
@@ -6294,27 +6294,27 @@
         <v>6075</v>
       </c>
       <c r="D137">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E137" t="s">
-        <v>164</v>
+        <v>103</v>
       </c>
       <c r="F137" t="s">
         <v>280</v>
       </c>
       <c r="G137" t="s">
-        <v>371</v>
+        <v>13</v>
       </c>
       <c r="H137" t="s">
         <v>280</v>
       </c>
       <c r="I137" t="s">
-        <v>19</v>
+        <v>280</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A138">
-        <v>6077</v>
+        <v>6078</v>
       </c>
       <c r="B138">
         <v>200</v>
@@ -6323,10 +6323,10 @@
         <v>6075</v>
       </c>
       <c r="D138">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E138" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="F138" t="s">
         <v>280</v>
@@ -6343,7 +6343,7 @@
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A139">
-        <v>6078</v>
+        <v>6079</v>
       </c>
       <c r="B139">
         <v>200</v>
@@ -6352,10 +6352,10 @@
         <v>6075</v>
       </c>
       <c r="D139">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E139" t="s">
-        <v>91</v>
+        <v>152</v>
       </c>
       <c r="F139" t="s">
         <v>280</v>
@@ -6372,7 +6372,7 @@
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A140">
-        <v>6079</v>
+        <v>6080</v>
       </c>
       <c r="B140">
         <v>200</v>
@@ -6381,10 +6381,10 @@
         <v>6075</v>
       </c>
       <c r="D140">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E140" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="F140" t="s">
         <v>280</v>
@@ -6401,7 +6401,7 @@
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A141">
-        <v>6080</v>
+        <v>6081</v>
       </c>
       <c r="B141">
         <v>200</v>
@@ -6410,10 +6410,10 @@
         <v>6075</v>
       </c>
       <c r="D141">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E141" t="s">
-        <v>156</v>
+        <v>92</v>
       </c>
       <c r="F141" t="s">
         <v>280</v>
@@ -6430,7 +6430,7 @@
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A142">
-        <v>6081</v>
+        <v>6082</v>
       </c>
       <c r="B142">
         <v>200</v>
@@ -6439,27 +6439,27 @@
         <v>6075</v>
       </c>
       <c r="D142">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E142" t="s">
-        <v>92</v>
+        <v>124</v>
       </c>
       <c r="F142" t="s">
         <v>280</v>
       </c>
-      <c r="G142" t="s">
-        <v>13</v>
+      <c r="G142" s="14" t="s">
+        <v>387</v>
       </c>
       <c r="H142" t="s">
         <v>280</v>
       </c>
       <c r="I142" t="s">
-        <v>280</v>
+        <v>19</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A143">
-        <v>6082</v>
+        <v>6083</v>
       </c>
       <c r="B143">
         <v>200</v>
@@ -6468,27 +6468,27 @@
         <v>6075</v>
       </c>
       <c r="D143">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E143" t="s">
-        <v>124</v>
+        <v>160</v>
       </c>
       <c r="F143" t="s">
         <v>280</v>
       </c>
-      <c r="G143" s="14" t="s">
-        <v>387</v>
+      <c r="G143" t="s">
+        <v>13</v>
       </c>
       <c r="H143" t="s">
         <v>280</v>
       </c>
       <c r="I143" t="s">
-        <v>19</v>
+        <v>280</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A144">
-        <v>6083</v>
+        <v>6084</v>
       </c>
       <c r="B144">
         <v>200</v>
@@ -6497,10 +6497,10 @@
         <v>6075</v>
       </c>
       <c r="D144">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E144" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="F144" t="s">
         <v>280</v>
@@ -6516,66 +6516,66 @@
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A145">
-        <v>6084</v>
-      </c>
-      <c r="B145">
-        <v>200</v>
-      </c>
-      <c r="C145">
-        <v>6075</v>
-      </c>
-      <c r="D145">
-        <v>9</v>
-      </c>
-      <c r="E145" t="s">
-        <v>172</v>
-      </c>
-      <c r="F145" t="s">
-        <v>280</v>
-      </c>
-      <c r="G145" t="s">
-        <v>13</v>
-      </c>
-      <c r="H145" t="s">
-        <v>280</v>
-      </c>
-      <c r="I145" t="s">
+      <c r="A145" s="6">
+        <v>6085</v>
+      </c>
+      <c r="B145" s="6">
+        <v>200</v>
+      </c>
+      <c r="C145" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="D145" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="E145" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="F145" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="G145" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H145" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="I145" s="6" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A146" s="6">
+      <c r="A146">
+        <v>6086</v>
+      </c>
+      <c r="B146">
+        <v>200</v>
+      </c>
+      <c r="C146">
         <v>6085</v>
       </c>
-      <c r="B146" s="6">
-        <v>200</v>
-      </c>
-      <c r="C146" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="D146" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="E146" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="F146" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G146" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H146" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I146" s="6" t="s">
+      <c r="D146">
+        <v>1</v>
+      </c>
+      <c r="E146" t="s">
+        <v>148</v>
+      </c>
+      <c r="F146" t="s">
+        <v>280</v>
+      </c>
+      <c r="G146" t="s">
+        <v>13</v>
+      </c>
+      <c r="H146" t="s">
+        <v>280</v>
+      </c>
+      <c r="I146" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A147">
-        <v>6086</v>
+        <v>6087</v>
       </c>
       <c r="B147">
         <v>200</v>
@@ -6584,10 +6584,10 @@
         <v>6085</v>
       </c>
       <c r="D147">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E147" t="s">
-        <v>148</v>
+        <v>176</v>
       </c>
       <c r="F147" t="s">
         <v>280</v>
@@ -6604,7 +6604,7 @@
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A148">
-        <v>6087</v>
+        <v>6088</v>
       </c>
       <c r="B148">
         <v>200</v>
@@ -6613,10 +6613,10 @@
         <v>6085</v>
       </c>
       <c r="D148">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E148" t="s">
-        <v>176</v>
+        <v>150</v>
       </c>
       <c r="F148" t="s">
         <v>280</v>
@@ -6633,7 +6633,7 @@
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A149">
-        <v>6088</v>
+        <v>6089</v>
       </c>
       <c r="B149">
         <v>200</v>
@@ -6642,10 +6642,10 @@
         <v>6085</v>
       </c>
       <c r="D149">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E149" t="s">
-        <v>150</v>
+        <v>173</v>
       </c>
       <c r="F149" t="s">
         <v>280</v>
@@ -6662,7 +6662,7 @@
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A150">
-        <v>6089</v>
+        <v>6090</v>
       </c>
       <c r="B150">
         <v>200</v>
@@ -6671,10 +6671,10 @@
         <v>6085</v>
       </c>
       <c r="D150">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E150" t="s">
-        <v>173</v>
+        <v>108</v>
       </c>
       <c r="F150" t="s">
         <v>280</v>
@@ -6691,7 +6691,7 @@
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A151">
-        <v>6090</v>
+        <v>6091</v>
       </c>
       <c r="B151">
         <v>200</v>
@@ -6700,10 +6700,10 @@
         <v>6085</v>
       </c>
       <c r="D151">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E151" t="s">
-        <v>108</v>
+        <v>146</v>
       </c>
       <c r="F151" t="s">
         <v>280</v>
@@ -6720,7 +6720,7 @@
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A152">
-        <v>6091</v>
+        <v>6092</v>
       </c>
       <c r="B152">
         <v>200</v>
@@ -6729,10 +6729,10 @@
         <v>6085</v>
       </c>
       <c r="D152">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E152" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="F152" t="s">
         <v>280</v>
@@ -6749,7 +6749,7 @@
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A153">
-        <v>6092</v>
+        <v>6093</v>
       </c>
       <c r="B153">
         <v>200</v>
@@ -6758,10 +6758,10 @@
         <v>6085</v>
       </c>
       <c r="D153">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E153" t="s">
-        <v>155</v>
+        <v>199</v>
       </c>
       <c r="F153" t="s">
         <v>280</v>
@@ -6778,7 +6778,7 @@
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A154">
-        <v>6093</v>
+        <v>6094</v>
       </c>
       <c r="B154">
         <v>200</v>
@@ -6787,10 +6787,10 @@
         <v>6085</v>
       </c>
       <c r="D154">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E154" t="s">
-        <v>199</v>
+        <v>115</v>
       </c>
       <c r="F154" t="s">
         <v>280</v>
@@ -6807,7 +6807,7 @@
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A155">
-        <v>6094</v>
+        <v>6095</v>
       </c>
       <c r="B155">
         <v>200</v>
@@ -6816,10 +6816,10 @@
         <v>6085</v>
       </c>
       <c r="D155">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E155" t="s">
-        <v>115</v>
+        <v>178</v>
       </c>
       <c r="F155" t="s">
         <v>280</v>
@@ -6836,7 +6836,7 @@
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A156">
-        <v>6095</v>
+        <v>6096</v>
       </c>
       <c r="B156">
         <v>200</v>
@@ -6845,10 +6845,10 @@
         <v>6085</v>
       </c>
       <c r="D156">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E156" t="s">
-        <v>178</v>
+        <v>94</v>
       </c>
       <c r="F156" t="s">
         <v>280</v>
@@ -6864,66 +6864,66 @@
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A157">
-        <v>6096</v>
-      </c>
-      <c r="B157">
-        <v>200</v>
-      </c>
-      <c r="C157">
-        <v>6085</v>
-      </c>
-      <c r="D157">
-        <v>11</v>
-      </c>
-      <c r="E157" t="s">
-        <v>94</v>
-      </c>
-      <c r="F157" t="s">
-        <v>280</v>
-      </c>
-      <c r="G157" t="s">
-        <v>13</v>
-      </c>
-      <c r="H157" t="s">
-        <v>280</v>
-      </c>
-      <c r="I157" t="s">
-        <v>280</v>
+      <c r="A157" s="6">
+        <v>6097</v>
+      </c>
+      <c r="B157" s="6">
+        <v>200</v>
+      </c>
+      <c r="C157" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="D157" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="E157" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="F157" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="G157" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H157" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="I157" s="6" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A158" s="6">
+      <c r="A158">
+        <v>6098</v>
+      </c>
+      <c r="B158">
+        <v>200</v>
+      </c>
+      <c r="C158">
         <v>6097</v>
       </c>
-      <c r="B158" s="6">
-        <v>200</v>
-      </c>
-      <c r="C158" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="D158" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="E158" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="F158" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G158" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H158" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I158" s="6" t="s">
-        <v>208</v>
+      <c r="D158">
+        <v>1</v>
+      </c>
+      <c r="E158" t="s">
+        <v>149</v>
+      </c>
+      <c r="F158" t="s">
+        <v>280</v>
+      </c>
+      <c r="G158" t="s">
+        <v>13</v>
+      </c>
+      <c r="H158" t="s">
+        <v>280</v>
+      </c>
+      <c r="I158" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A159">
-        <v>6098</v>
+        <v>6099</v>
       </c>
       <c r="B159">
         <v>200</v>
@@ -6932,10 +6932,10 @@
         <v>6097</v>
       </c>
       <c r="D159">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E159" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="F159" t="s">
         <v>280</v>
@@ -6952,7 +6952,7 @@
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A160">
-        <v>6099</v>
+        <v>6100</v>
       </c>
       <c r="B160">
         <v>200</v>
@@ -6961,10 +6961,10 @@
         <v>6097</v>
       </c>
       <c r="D160">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E160" t="s">
-        <v>141</v>
+        <v>177</v>
       </c>
       <c r="F160" t="s">
         <v>280</v>
@@ -6981,7 +6981,7 @@
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A161">
-        <v>6100</v>
+        <v>6101</v>
       </c>
       <c r="B161">
         <v>200</v>
@@ -6990,10 +6990,10 @@
         <v>6097</v>
       </c>
       <c r="D161">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E161" t="s">
-        <v>177</v>
+        <v>145</v>
       </c>
       <c r="F161" t="s">
         <v>280</v>
@@ -7010,7 +7010,7 @@
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A162">
-        <v>6101</v>
+        <v>6102</v>
       </c>
       <c r="B162">
         <v>200</v>
@@ -7019,27 +7019,27 @@
         <v>6097</v>
       </c>
       <c r="D162">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E162" t="s">
-        <v>145</v>
+        <v>175</v>
       </c>
       <c r="F162" t="s">
         <v>280</v>
       </c>
       <c r="G162" t="s">
-        <v>13</v>
+        <v>315</v>
       </c>
       <c r="H162" t="s">
         <v>280</v>
       </c>
       <c r="I162" t="s">
-        <v>280</v>
+        <v>19</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A163">
-        <v>6102</v>
+        <v>6103</v>
       </c>
       <c r="B163">
         <v>200</v>
@@ -7048,27 +7048,27 @@
         <v>6097</v>
       </c>
       <c r="D163">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E163" t="s">
-        <v>175</v>
+        <v>138</v>
       </c>
       <c r="F163" t="s">
         <v>280</v>
       </c>
       <c r="G163" t="s">
-        <v>315</v>
+        <v>13</v>
       </c>
       <c r="H163" t="s">
         <v>280</v>
       </c>
       <c r="I163" t="s">
-        <v>19</v>
+        <v>280</v>
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A164">
-        <v>6103</v>
+        <v>6104</v>
       </c>
       <c r="B164">
         <v>200</v>
@@ -7077,10 +7077,10 @@
         <v>6097</v>
       </c>
       <c r="D164">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E164" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="F164" t="s">
         <v>280</v>
@@ -7097,7 +7097,7 @@
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A165">
-        <v>6104</v>
+        <v>6105</v>
       </c>
       <c r="B165">
         <v>200</v>
@@ -7106,27 +7106,27 @@
         <v>6097</v>
       </c>
       <c r="D165">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E165" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="F165" t="s">
         <v>280</v>
       </c>
       <c r="G165" t="s">
-        <v>13</v>
+        <v>388</v>
       </c>
       <c r="H165" t="s">
         <v>280</v>
       </c>
       <c r="I165" t="s">
-        <v>280</v>
+        <v>19</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A166">
-        <v>6105</v>
+        <v>6106</v>
       </c>
       <c r="B166">
         <v>200</v>
@@ -7135,27 +7135,27 @@
         <v>6097</v>
       </c>
       <c r="D166">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E166" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F166" t="s">
         <v>280</v>
       </c>
-      <c r="G166" s="14" t="s">
-        <v>388</v>
+      <c r="G166" t="s">
+        <v>13</v>
       </c>
       <c r="H166" t="s">
         <v>280</v>
       </c>
       <c r="I166" t="s">
-        <v>19</v>
+        <v>280</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A167">
-        <v>6106</v>
+        <v>6107</v>
       </c>
       <c r="B167">
         <v>200</v>
@@ -7164,10 +7164,10 @@
         <v>6097</v>
       </c>
       <c r="D167">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E167" t="s">
-        <v>114</v>
+        <v>174</v>
       </c>
       <c r="F167" t="s">
         <v>280</v>
@@ -7184,7 +7184,7 @@
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A168">
-        <v>6107</v>
+        <v>6108</v>
       </c>
       <c r="B168">
         <v>200</v>
@@ -7193,59 +7193,59 @@
         <v>6097</v>
       </c>
       <c r="D168">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E168" t="s">
-        <v>174</v>
+        <v>143</v>
       </c>
       <c r="F168" t="s">
         <v>280</v>
       </c>
       <c r="G168" t="s">
-        <v>13</v>
+        <v>311</v>
       </c>
       <c r="H168" t="s">
         <v>280</v>
       </c>
       <c r="I168" t="s">
-        <v>280</v>
+        <v>19</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A169">
-        <v>6108</v>
-      </c>
-      <c r="B169">
-        <v>200</v>
-      </c>
-      <c r="C169">
-        <v>6097</v>
-      </c>
-      <c r="D169">
-        <v>11</v>
-      </c>
-      <c r="E169" t="s">
-        <v>143</v>
-      </c>
-      <c r="F169" t="s">
-        <v>280</v>
-      </c>
-      <c r="G169" t="s">
-        <v>311</v>
-      </c>
-      <c r="H169" t="s">
-        <v>280</v>
-      </c>
-      <c r="I169" t="s">
-        <v>19</v>
+      <c r="A169" s="14">
+        <v>600200</v>
+      </c>
+      <c r="B169" s="14">
+        <v>6002</v>
+      </c>
+      <c r="C169" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="D169" s="14">
+        <v>1</v>
+      </c>
+      <c r="E169" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="F169" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="G169" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="H169" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="I169" s="14" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A170" s="14">
-        <v>600200</v>
+        <v>603600</v>
       </c>
       <c r="B170" s="14">
-        <v>6002</v>
+        <v>6036</v>
       </c>
       <c r="C170" s="14" t="s">
         <v>280</v>
@@ -7254,13 +7254,13 @@
         <v>1</v>
       </c>
       <c r="E170" s="14" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="F170" s="14" t="s">
         <v>185</v>
       </c>
       <c r="G170" s="14" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="H170" s="14" t="s">
         <v>12</v>
@@ -7271,10 +7271,10 @@
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A171" s="14">
-        <v>603600</v>
+        <v>604300</v>
       </c>
       <c r="B171" s="14">
-        <v>6036</v>
+        <v>6043</v>
       </c>
       <c r="C171" s="14" t="s">
         <v>280</v>
@@ -7283,13 +7283,13 @@
         <v>1</v>
       </c>
       <c r="E171" s="14" t="s">
-        <v>250</v>
+        <v>215</v>
       </c>
       <c r="F171" s="14" t="s">
         <v>185</v>
       </c>
       <c r="G171" s="14" t="s">
-        <v>254</v>
+        <v>291</v>
       </c>
       <c r="H171" s="14" t="s">
         <v>12</v>
@@ -7300,10 +7300,10 @@
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A172" s="14">
-        <v>604300</v>
+        <v>605300</v>
       </c>
       <c r="B172" s="14">
-        <v>6043</v>
+        <v>6053</v>
       </c>
       <c r="C172" s="14" t="s">
         <v>280</v>
@@ -7312,13 +7312,13 @@
         <v>1</v>
       </c>
       <c r="E172" s="14" t="s">
-        <v>215</v>
+        <v>278</v>
       </c>
       <c r="F172" s="14" t="s">
         <v>185</v>
       </c>
       <c r="G172" s="14" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="H172" s="14" t="s">
         <v>12</v>
@@ -7329,10 +7329,10 @@
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A173" s="14">
-        <v>605300</v>
+        <v>605600</v>
       </c>
       <c r="B173" s="14">
-        <v>6053</v>
+        <v>6056</v>
       </c>
       <c r="C173" s="14" t="s">
         <v>280</v>
@@ -7341,13 +7341,13 @@
         <v>1</v>
       </c>
       <c r="E173" s="14" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="F173" s="14" t="s">
         <v>185</v>
       </c>
       <c r="G173" s="14" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="H173" s="14" t="s">
         <v>12</v>
@@ -7358,10 +7358,10 @@
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A174" s="14">
-        <v>605600</v>
+        <v>606500</v>
       </c>
       <c r="B174" s="14">
-        <v>6056</v>
+        <v>6065</v>
       </c>
       <c r="C174" s="14" t="s">
         <v>280</v>
@@ -7370,13 +7370,13 @@
         <v>1</v>
       </c>
       <c r="E174" s="14" t="s">
-        <v>271</v>
+        <v>1</v>
       </c>
       <c r="F174" s="14" t="s">
         <v>185</v>
       </c>
       <c r="G174" s="14" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="H174" s="14" t="s">
         <v>12</v>
@@ -7387,10 +7387,10 @@
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A175" s="14">
-        <v>606500</v>
+        <v>607100</v>
       </c>
       <c r="B175" s="14">
-        <v>6065</v>
+        <v>6071</v>
       </c>
       <c r="C175" s="14" t="s">
         <v>280</v>
@@ -7399,13 +7399,13 @@
         <v>1</v>
       </c>
       <c r="E175" s="14" t="s">
-        <v>1</v>
+        <v>219</v>
       </c>
       <c r="F175" s="14" t="s">
         <v>185</v>
       </c>
       <c r="G175" s="14" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="H175" s="14" t="s">
         <v>12</v>
@@ -7416,10 +7416,10 @@
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A176" s="14">
-        <v>607100</v>
+        <v>610800</v>
       </c>
       <c r="B176" s="14">
-        <v>6071</v>
+        <v>6108</v>
       </c>
       <c r="C176" s="14" t="s">
         <v>280</v>
@@ -7428,13 +7428,13 @@
         <v>1</v>
       </c>
       <c r="E176" s="14" t="s">
-        <v>219</v>
+        <v>274</v>
       </c>
       <c r="F176" s="14" t="s">
         <v>185</v>
       </c>
       <c r="G176" s="14" t="s">
-        <v>295</v>
+        <v>311</v>
       </c>
       <c r="H176" s="14" t="s">
         <v>12</v>
@@ -7445,10 +7445,10 @@
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A177" s="14">
-        <v>610800</v>
+        <v>605900</v>
       </c>
       <c r="B177" s="14">
-        <v>6108</v>
+        <v>6059</v>
       </c>
       <c r="C177" s="14" t="s">
         <v>280</v>
@@ -7457,13 +7457,13 @@
         <v>1</v>
       </c>
       <c r="E177" s="14" t="s">
-        <v>274</v>
+        <v>316</v>
       </c>
       <c r="F177" s="14" t="s">
         <v>185</v>
       </c>
       <c r="G177" s="14" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="H177" s="14" t="s">
         <v>12</v>
@@ -7474,10 +7474,10 @@
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A178" s="14">
-        <v>605900</v>
+        <v>605200</v>
       </c>
       <c r="B178" s="14">
-        <v>6059</v>
+        <v>6052</v>
       </c>
       <c r="C178" s="14" t="s">
         <v>280</v>
@@ -7486,13 +7486,13 @@
         <v>1</v>
       </c>
       <c r="E178" s="14" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="F178" s="14" t="s">
         <v>185</v>
       </c>
       <c r="G178" s="14" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="H178" s="14" t="s">
         <v>12</v>
@@ -7503,10 +7503,10 @@
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A179" s="14">
-        <v>605200</v>
+        <v>607400</v>
       </c>
       <c r="B179" s="14">
-        <v>6052</v>
+        <v>6074</v>
       </c>
       <c r="C179" s="14" t="s">
         <v>280</v>
@@ -7515,13 +7515,13 @@
         <v>1</v>
       </c>
       <c r="E179" s="14" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="F179" s="14" t="s">
         <v>185</v>
       </c>
       <c r="G179" s="14" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="H179" s="14" t="s">
         <v>12</v>
@@ -7532,10 +7532,10 @@
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A180" s="14">
-        <v>607400</v>
+        <v>610200</v>
       </c>
       <c r="B180" s="14">
-        <v>6074</v>
+        <v>6102</v>
       </c>
       <c r="C180" s="14" t="s">
         <v>280</v>
@@ -7544,13 +7544,13 @@
         <v>1</v>
       </c>
       <c r="E180" s="14" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="F180" s="14" t="s">
         <v>185</v>
       </c>
       <c r="G180" s="14" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="H180" s="14" t="s">
         <v>12</v>
@@ -7561,10 +7561,10 @@
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A181" s="14">
-        <v>610200</v>
+        <v>607600</v>
       </c>
       <c r="B181" s="14">
-        <v>6102</v>
+        <v>6076</v>
       </c>
       <c r="C181" s="14" t="s">
         <v>280</v>
@@ -7573,13 +7573,13 @@
         <v>1</v>
       </c>
       <c r="E181" s="14" t="s">
-        <v>319</v>
+        <v>372</v>
       </c>
       <c r="F181" s="14" t="s">
         <v>185</v>
       </c>
       <c r="G181" s="14" t="s">
-        <v>315</v>
+        <v>371</v>
       </c>
       <c r="H181" s="14" t="s">
         <v>12</v>
@@ -7590,10 +7590,10 @@
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A182" s="14">
-        <v>607600</v>
+        <v>600800</v>
       </c>
       <c r="B182" s="14">
-        <v>6076</v>
+        <v>6008</v>
       </c>
       <c r="C182" s="14" t="s">
         <v>280</v>
@@ -7602,13 +7602,13 @@
         <v>1</v>
       </c>
       <c r="E182" s="14" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c r="F182" s="14" t="s">
         <v>185</v>
       </c>
       <c r="G182" s="14" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="H182" s="14" t="s">
         <v>12</v>
@@ -7619,10 +7619,10 @@
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A183" s="14">
-        <v>600800</v>
+        <v>603300</v>
       </c>
       <c r="B183" s="14">
-        <v>6008</v>
+        <v>6033</v>
       </c>
       <c r="C183" s="14" t="s">
         <v>280</v>
@@ -7631,13 +7631,13 @@
         <v>1</v>
       </c>
       <c r="E183" s="14" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="F183" s="14" t="s">
         <v>185</v>
       </c>
       <c r="G183" s="14" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="H183" s="14" t="s">
         <v>12</v>
@@ -7648,10 +7648,10 @@
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A184" s="14">
-        <v>603300</v>
+        <v>602500</v>
       </c>
       <c r="B184" s="14">
-        <v>6033</v>
+        <v>6025</v>
       </c>
       <c r="C184" s="14" t="s">
         <v>280</v>
@@ -7660,13 +7660,13 @@
         <v>1</v>
       </c>
       <c r="E184" s="14" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="F184" s="14" t="s">
         <v>185</v>
       </c>
       <c r="G184" s="14" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="H184" s="14" t="s">
         <v>12</v>
@@ -7677,10 +7677,10 @@
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A185" s="14">
-        <v>602500</v>
+        <v>607000</v>
       </c>
       <c r="B185" s="14">
-        <v>6025</v>
+        <v>6070</v>
       </c>
       <c r="C185" s="14" t="s">
         <v>280</v>
@@ -7689,13 +7689,13 @@
         <v>1</v>
       </c>
       <c r="E185" s="14" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="F185" s="14" t="s">
         <v>185</v>
       </c>
       <c r="G185" s="14" t="s">
-        <v>381</v>
+        <v>386</v>
       </c>
       <c r="H185" s="14" t="s">
         <v>12</v>
@@ -7706,10 +7706,10 @@
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A186" s="14">
-        <v>607000</v>
+        <v>608200</v>
       </c>
       <c r="B186" s="14">
-        <v>6070</v>
+        <v>6082</v>
       </c>
       <c r="C186" s="14" t="s">
         <v>280</v>
@@ -7718,13 +7718,13 @@
         <v>1</v>
       </c>
       <c r="E186" s="14" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="F186" s="14" t="s">
         <v>185</v>
       </c>
       <c r="G186" s="14" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="H186" s="14" t="s">
         <v>12</v>
@@ -7735,10 +7735,10 @@
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A187" s="14">
-        <v>608200</v>
+        <v>610500</v>
       </c>
       <c r="B187" s="14">
-        <v>6082</v>
+        <v>6105</v>
       </c>
       <c r="C187" s="14" t="s">
         <v>280</v>
@@ -7747,47 +7747,18 @@
         <v>1</v>
       </c>
       <c r="E187" s="14" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="F187" s="14" t="s">
         <v>185</v>
       </c>
       <c r="G187" s="14" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="H187" s="14" t="s">
         <v>12</v>
       </c>
       <c r="I187" s="14" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A188" s="14">
-        <v>610500</v>
-      </c>
-      <c r="B188" s="14">
-        <v>6105</v>
-      </c>
-      <c r="C188" s="14" t="s">
-        <v>280</v>
-      </c>
-      <c r="D188" s="14">
-        <v>1</v>
-      </c>
-      <c r="E188" s="14" t="s">
-        <v>385</v>
-      </c>
-      <c r="F188" s="14" t="s">
-        <v>185</v>
-      </c>
-      <c r="G188" s="14" t="s">
-        <v>388</v>
-      </c>
-      <c r="H188" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="I188" s="14" t="s">
         <v>212</v>
       </c>
     </row>
@@ -7804,7 +7775,7 @@
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8236,11 +8207,11 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:I238"/>
+  <dimension ref="A1:I240"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A136" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E226" sqref="E226:E238"/>
+      <pane ySplit="1" topLeftCell="A224" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E252" sqref="E252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14041,6 +14012,35 @@
         <v>19</v>
       </c>
     </row>
+    <row r="240" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A240" s="5">
+        <v>5130</v>
+      </c>
+      <c r="B240" s="5">
+        <v>100</v>
+      </c>
+      <c r="C240" s="5">
+        <v>5000</v>
+      </c>
+      <c r="D240" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="E240" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="F240" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="G240" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="H240" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I240" s="5" t="s">
+        <v>208</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G17" r:id="rId1"/>

</xml_diff>